<commit_message>
Work for the day ⌛ Small correction to install packages script Small change in paragraph spacing
</commit_message>
<xml_diff>
--- a/papers/stats/stats_spreadsheet.xlsx
+++ b/papers/stats/stats_spreadsheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="39">
   <si>
     <t>Paper Title</t>
   </si>
@@ -42,12 +42,21 @@
     <t>Psycholinguistic aspects of pauses and temporal patterns in schizophrenic speech</t>
   </si>
   <si>
+    <t>Process and Reactive Schizophrenia: Some Conceptions and Issues</t>
+  </si>
+  <si>
     <t>Clemmer, Edward J.</t>
   </si>
   <si>
+    <t>Garmezy N</t>
+  </si>
+  <si>
     <t>1980</t>
   </si>
   <si>
+    <t>Fall 1970</t>
+  </si>
+  <si>
     <t>Gibberish</t>
   </si>
   <si>
@@ -124,6 +133,9 @@
   </si>
   <si>
     <t>Classifying Schizophrenic</t>
+  </si>
+  <si>
+    <t>Diagnosis by Prognosis</t>
   </si>
 </sst>
 </file>
@@ -488,7 +500,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
@@ -503,7 +515,7 @@
     <col min="3" max="3" width="20.5703125" customWidth="1"/>
     <col min="4" max="4" width="11.7109375" customWidth="1"/>
     <col min="5" max="5" width="11.7109375" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" customWidth="1"/>
     <col min="7" max="7" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -535,10 +547,10 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E2" s="2">
         <v>44460</v>
@@ -548,6 +560,29 @@
       </c>
       <c r="G2">
         <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="2">
+        <v>44466</v>
+      </c>
+      <c r="F3" s="2">
+        <v>2958465</v>
+      </c>
+      <c r="G3">
+        <v>2913999</v>
       </c>
     </row>
   </sheetData>
@@ -557,7 +592,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
@@ -583,25 +618,25 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -631,6 +666,14 @@
       </c>
       <c r="I2" s="3">
         <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -640,7 +683,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
@@ -663,16 +706,16 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -693,6 +736,14 @@
       </c>
       <c r="F2" s="3">
         <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -702,7 +753,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
@@ -729,28 +780,28 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -761,28 +812,36 @@
         <v>6</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -792,7 +851,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
@@ -816,19 +875,19 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -839,19 +898,27 @@
         <v>6</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -861,7 +928,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
@@ -874,17 +941,21 @@
   <cols>
     <col min="2" max="2" width="88.7109375" customWidth="1"/>
     <col min="3" max="3" width="28.28515625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="24.85546875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>37</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -892,7 +963,18 @@
         <v>6</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Work for the day ⌛ Also changed scoring for parameters with score from -1 to +1 float
</commit_message>
<xml_diff>
--- a/papers/stats/stats_spreadsheet.xlsx
+++ b/papers/stats/stats_spreadsheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="46">
   <si>
     <t>Paper Title</t>
   </si>
@@ -45,22 +45,31 @@
     <t>Process and Reactive Schizophrenia: Some Conceptions and Issues</t>
   </si>
   <si>
+    <t>Thought disorder or speech disorder in schizophrenia?</t>
+  </si>
+  <si>
     <t>Clemmer, Edward J.</t>
   </si>
   <si>
     <t>Garmezy N</t>
   </si>
   <si>
+    <t>Chaika E.</t>
+  </si>
+  <si>
     <t>1980</t>
   </si>
   <si>
     <t>Fall 1970</t>
   </si>
   <si>
+    <t>1982</t>
+  </si>
+  <si>
     <t>Gibberish</t>
   </si>
   <si>
-    <t>Absnormal Rhyming</t>
+    <t>Abnormal Rhyming</t>
   </si>
   <si>
     <t>Absence of Topic</t>
@@ -78,6 +87,15 @@
     <t>Disruption on Flow of Ideas</t>
   </si>
   <si>
+    <t>Neologization</t>
+  </si>
+  <si>
+    <t>Word Salad</t>
+  </si>
+  <si>
+    <t>Aliteration</t>
+  </si>
+  <si>
     <t>Matching of Control with Schizophrenic</t>
   </si>
   <si>
@@ -129,13 +147,16 @@
     <t>Schizophrenic under Lobotomy</t>
   </si>
   <si>
-    <t>Difference with other Neurological Disorder</t>
+    <t>Difference with other Neurological Disorders</t>
   </si>
   <si>
     <t>Classifying Schizophrenic</t>
   </si>
   <si>
     <t>Diagnosis by Prognosis</t>
+  </si>
+  <si>
+    <t>Thought Disorder VS Speech Disorder</t>
   </si>
 </sst>
 </file>
@@ -500,7 +521,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
@@ -547,10 +568,10 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E2" s="2">
         <v>44460</v>
@@ -570,10 +591,10 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E3" s="2">
         <v>44466</v>
@@ -583,6 +604,29 @@
       </c>
       <c r="G3">
         <v>2913999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="2">
+        <v>44466</v>
+      </c>
+      <c r="F4" s="2">
+        <v>44466</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -592,7 +636,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
@@ -605,41 +649,53 @@
   <cols>
     <col min="2" max="2" width="88.7109375" customWidth="1"/>
     <col min="3" max="3" width="10.5703125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" style="3" customWidth="1"/>
     <col min="5" max="5" width="18.28515625" style="3" customWidth="1"/>
     <col min="6" max="6" width="29.28515625" style="3" customWidth="1"/>
     <col min="7" max="7" width="34.85546875" style="3" customWidth="1"/>
     <col min="8" max="8" width="29.28515625" style="3" customWidth="1"/>
     <col min="9" max="9" width="30.42578125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="15" style="3" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" style="3" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:12">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+        <v>21</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -650,30 +706,53 @@
         <v>1</v>
       </c>
       <c r="D2" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="F2" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G2" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="H2" s="3">
+        <v>-0.5</v>
+      </c>
+      <c r="I2" s="3">
         <v>1</v>
       </c>
-      <c r="E2" s="3">
-        <v>1</v>
-      </c>
-      <c r="F2" s="3">
-        <v>1</v>
-      </c>
-      <c r="G2" s="3">
-        <v>1</v>
-      </c>
-      <c r="H2" s="3">
-        <v>-1</v>
-      </c>
-      <c r="I2" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="J4" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="K4" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="L4" s="3">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>
@@ -683,7 +762,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
@@ -706,16 +785,16 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -726,16 +805,16 @@
         <v>6</v>
       </c>
       <c r="C2" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D2" s="3">
         <v>1</v>
       </c>
-      <c r="D2" s="3">
-        <v>2</v>
-      </c>
       <c r="E2" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F2" s="3">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -744,6 +823,14 @@
       </c>
       <c r="B3" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -753,7 +840,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
@@ -780,28 +867,28 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -812,28 +899,28 @@
         <v>6</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -842,6 +929,14 @@
       </c>
       <c r="B3" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -851,7 +946,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
@@ -867,7 +962,7 @@
     <col min="4" max="4" width="13.85546875" style="3" customWidth="1"/>
     <col min="5" max="5" width="33.7109375" style="3" customWidth="1"/>
     <col min="6" max="6" width="31.5703125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="48" style="3" customWidth="1"/>
+    <col min="7" max="7" width="49.140625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -875,19 +970,19 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -898,19 +993,19 @@
         <v>6</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -919,6 +1014,17 @@
       </c>
       <c r="B3" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -928,7 +1034,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
@@ -942,20 +1048,24 @@
     <col min="2" max="2" width="88.7109375" customWidth="1"/>
     <col min="3" max="3" width="28.28515625" style="3" customWidth="1"/>
     <col min="4" max="4" width="24.85546875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="39.28515625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+        <v>44</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -963,10 +1073,10 @@
         <v>6</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -974,7 +1084,18 @@
         <v>7</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>31</v>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created first Paper Critique 🎉 Created script for initializing a template Changed python code for spreadsheet now it displays count, sum and mean
</commit_message>
<xml_diff>
--- a/papers/stats/stats_spreadsheet.xlsx
+++ b/papers/stats/stats_spreadsheet.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rodrigo\Desktop\Repos\PMEIC-2122\papers\stats\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3F7CA7D-56E0-4014-B077-DF1B70EA7BD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -14,12 +20,12 @@
     <sheet name="Problems" sheetId="5" r:id="rId5"/>
     <sheet name="Citations" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="49">
   <si>
     <t>Paper Title</t>
   </si>
@@ -96,6 +102,12 @@
     <t>Aliteration</t>
   </si>
   <si>
+    <t>Sum Value</t>
+  </si>
+  <si>
+    <t>Mean Value</t>
+  </si>
+  <si>
     <t>Matching of Control with Schizophrenic</t>
   </si>
   <si>
@@ -133,6 +145,9 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>Count Times</t>
   </si>
   <si>
     <t>Restrictive Sample</t>
@@ -162,11 +177,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
-  </numFmts>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -223,7 +235,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -233,11 +245,19 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -279,7 +299,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -311,9 +331,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -345,6 +383,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -520,123 +576,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="2" max="2" width="88.7109375" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" customWidth="1"/>
-    <col min="6" max="6" width="21.5703125" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="2">
-        <v>44460</v>
-      </c>
-      <c r="F2" s="2">
-        <v>44462</v>
-      </c>
-      <c r="G2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="2">
-        <v>44466</v>
-      </c>
-      <c r="F3" s="2">
-        <v>2958465</v>
-      </c>
-      <c r="G3">
-        <v>2913999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="2">
-        <v>44466</v>
-      </c>
-      <c r="F4" s="2">
-        <v>44466</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
@@ -645,12 +586,125 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="88.7109375" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" customWidth="1"/>
+    <col min="4" max="5" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="2">
+        <v>44460</v>
+      </c>
+      <c r="F2" s="2">
+        <v>44462</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="2">
+        <v>44466</v>
+      </c>
+      <c r="F3" s="2">
+        <v>2958465</v>
+      </c>
+      <c r="G3">
+        <v>2913999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="2">
+        <v>44466</v>
+      </c>
+      <c r="F4" s="2">
+        <v>44466</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:L7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="88.7109375" customWidth="1"/>
     <col min="3" max="3" width="10.5703125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" style="3" customWidth="1"/>
+    <col min="4" max="5" width="18.28515625" style="3" customWidth="1"/>
     <col min="6" max="6" width="29.28515625" style="3" customWidth="1"/>
     <col min="7" max="7" width="34.85546875" style="3" customWidth="1"/>
     <col min="8" max="8" width="29.28515625" style="3" customWidth="1"/>
@@ -660,7 +714,7 @@
     <col min="12" max="12" width="12.85546875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -695,7 +749,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -724,7 +778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -732,7 +786,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -752,6 +806,76 @@
         <v>0.5</v>
       </c>
       <c r="L4" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="H6" s="3">
+        <v>-0.5</v>
+      </c>
+      <c r="I6" s="3">
+        <v>1</v>
+      </c>
+      <c r="J6" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="K6" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="L6" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="H7" s="3">
+        <v>-0.5</v>
+      </c>
+      <c r="I7" s="3">
+        <v>1</v>
+      </c>
+      <c r="J7" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="K7" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="L7" s="3">
         <v>0.5</v>
       </c>
     </row>
@@ -761,8 +885,8 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
@@ -771,7 +895,7 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="88.7109375" customWidth="1"/>
     <col min="3" max="3" width="42.5703125" style="3" customWidth="1"/>
@@ -780,24 +904,24 @@
     <col min="6" max="6" width="15" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -817,7 +941,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -825,12 +949,46 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>
@@ -839,8 +997,8 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
@@ -849,49 +1007,47 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="88.7109375" customWidth="1"/>
     <col min="3" max="3" width="17.28515625" style="3" customWidth="1"/>
     <col min="4" max="4" width="23.85546875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="27.140625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="27.140625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="27.140625" style="3" customWidth="1"/>
+    <col min="5" max="7" width="27.140625" style="3" customWidth="1"/>
     <col min="8" max="8" width="20.5703125" style="3" customWidth="1"/>
     <col min="9" max="9" width="26" style="3" customWidth="1"/>
     <col min="10" max="10" width="35.85546875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -899,31 +1055,31 @@
         <v>6</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -931,12 +1087,41 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1</v>
+      </c>
+      <c r="F6" s="3">
+        <v>1</v>
+      </c>
+      <c r="G6" s="3">
+        <v>1</v>
+      </c>
+      <c r="H6" s="3">
+        <v>1</v>
+      </c>
+      <c r="I6" s="3">
+        <v>1</v>
+      </c>
+      <c r="J6" s="3">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -945,8 +1130,8 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
@@ -955,7 +1140,7 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="88.7109375" customWidth="1"/>
     <col min="3" max="3" width="20.5703125" style="3" customWidth="1"/>
@@ -965,27 +1150,27 @@
     <col min="7" max="7" width="49.140625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -993,22 +1178,22 @@
         <v>6</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1016,7 +1201,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1024,7 +1209,27 @@
         <v>8</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1</v>
+      </c>
+      <c r="F6" s="3">
+        <v>1</v>
+      </c>
+      <c r="G6" s="3">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1033,17 +1238,17 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="88.7109375" customWidth="1"/>
     <col min="3" max="3" width="28.28515625" style="3" customWidth="1"/>
@@ -1051,21 +1256,21 @@
     <col min="5" max="5" width="39.28515625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1073,10 +1278,10 @@
         <v>6</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1084,10 +1289,10 @@
         <v>7</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1095,7 +1300,21 @@
         <v>8</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Work for the day ⌛ Added more packages into install Cleanup now cleans .out files
</commit_message>
<xml_diff>
--- a/papers/stats/stats_spreadsheet.xlsx
+++ b/papers/stats/stats_spreadsheet.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rodrigo\Desktop\Repos\PMEIC-2122\papers\stats\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3F7CA7D-56E0-4014-B077-DF1B70EA7BD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -20,12 +14,12 @@
     <sheet name="Problems" sheetId="5" r:id="rId5"/>
     <sheet name="Citations" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="63">
   <si>
     <t>Paper Title</t>
   </si>
@@ -45,6 +39,9 @@
     <t>Days Taken</t>
   </si>
   <si>
+    <t>Age-Related Differences in Formal Thought Disorderin Chronically Hospitalized Schizophrenic Patients:A Cross-Sectional Study Across Nine Decades</t>
+  </si>
+  <si>
     <t>Psycholinguistic aspects of pauses and temporal patterns in schizophrenic speech</t>
   </si>
   <si>
@@ -54,6 +51,9 @@
     <t>Thought disorder or speech disorder in schizophrenia?</t>
   </si>
   <si>
+    <t>Harvey F, Leibman L, Al E.</t>
+  </si>
+  <si>
     <t>Clemmer, Edward J.</t>
   </si>
   <si>
@@ -63,6 +63,9 @@
     <t>Chaika E.</t>
   </si>
   <si>
+    <t>1997</t>
+  </si>
+  <si>
     <t>1980</t>
   </si>
   <si>
@@ -72,6 +75,18 @@
     <t>1982</t>
   </si>
   <si>
+    <t>Poverty of Speech</t>
+  </si>
+  <si>
+    <t>Disruption on Flow of Ideas</t>
+  </si>
+  <si>
+    <t>Distractibility</t>
+  </si>
+  <si>
+    <t>Absence of Self Monitoring</t>
+  </si>
+  <si>
     <t>Gibberish</t>
   </si>
   <si>
@@ -87,12 +102,6 @@
     <t>Preoccupation with Syntax Rules</t>
   </si>
   <si>
-    <t>Absence of Self Monitoring</t>
-  </si>
-  <si>
-    <t>Disruption on Flow of Ideas</t>
-  </si>
-  <si>
     <t>Neologization</t>
   </si>
   <si>
@@ -108,6 +117,18 @@
     <t>Mean Value</t>
   </si>
   <si>
+    <t>Diagnostic Interview</t>
+  </si>
+  <si>
+    <t>Clinical History Chart Review</t>
+  </si>
+  <si>
+    <t>Open Interview</t>
+  </si>
+  <si>
+    <t>Open Interview with Caregivers</t>
+  </si>
+  <si>
     <t>Matching of Control with Schizophrenic</t>
   </si>
   <si>
@@ -120,6 +141,15 @@
     <t>Unusual Story</t>
   </si>
   <si>
+    <t>Scale  for  Assessment  of  Thought,  Language, and Communication</t>
+  </si>
+  <si>
+    <t>Mini-Mental  State  examination</t>
+  </si>
+  <si>
+    <t>DSM-III-R Criterion</t>
+  </si>
+  <si>
     <t>Speech Duration</t>
   </si>
   <si>
@@ -148,6 +178,12 @@
   </si>
   <si>
     <t>Count Times</t>
+  </si>
+  <si>
+    <t>No Control Group</t>
+  </si>
+  <si>
+    <t>Different Environments</t>
   </si>
   <si>
     <t>Restrictive Sample</t>
@@ -177,8 +213,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
+  </numFmts>
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -235,7 +274,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -245,19 +284,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -299,7 +330,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -331,27 +362,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -383,24 +396,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -576,26 +571,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="88.7109375" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" customWidth="1"/>
-    <col min="4" max="5" width="11.7109375" customWidth="1"/>
-    <col min="6" max="6" width="21.5703125" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="144.7109375" customWidth="1"/>
+    <col min="3" max="3" width="26.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -615,7 +611,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -623,22 +619,22 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E2" s="2">
-        <v>44460</v>
+        <v>44468</v>
       </c>
       <c r="F2" s="2">
-        <v>44462</v>
+        <v>44469</v>
       </c>
       <c r="G2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -646,22 +642,22 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E3" s="2">
-        <v>44466</v>
+        <v>44460</v>
       </c>
       <c r="F3" s="2">
-        <v>2958465</v>
+        <v>44462</v>
       </c>
       <c r="G3">
-        <v>2913999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -669,18 +665,41 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E4" s="2">
         <v>44466</v>
       </c>
       <c r="F4" s="2">
+        <v>2958465</v>
+      </c>
+      <c r="G4">
+        <v>2913999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="2">
         <v>44466</v>
       </c>
-      <c r="G4">
+      <c r="F5" s="2">
+        <v>44466</v>
+      </c>
+      <c r="G5">
         <v>0</v>
       </c>
     </row>
@@ -690,66 +709,75 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="88.7109375" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" style="3" customWidth="1"/>
-    <col min="4" max="5" width="18.28515625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="29.28515625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="34.85546875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="29.28515625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="30.42578125" style="3" customWidth="1"/>
-    <col min="10" max="10" width="15" style="3" customWidth="1"/>
-    <col min="11" max="11" width="11.7109375" style="3" customWidth="1"/>
-    <col min="12" max="12" width="12.85546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="144.7109375" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="27.7109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="26.7109375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" style="3" customWidth="1"/>
+    <col min="10" max="10" width="26.7109375" style="3" customWidth="1"/>
+    <col min="11" max="11" width="31.7109375" style="3" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" style="3" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" style="3" customWidth="1"/>
+    <col min="14" max="14" width="11.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -760,7 +788,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="3">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E2" s="3">
         <v>0.5</v>
@@ -768,114 +796,146 @@
       <c r="F2" s="3">
         <v>0.5</v>
       </c>
-      <c r="G2" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="H2" s="3">
-        <v>-0.5</v>
-      </c>
-      <c r="I2" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D3" s="3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3">
+        <v>-0.5</v>
+      </c>
+      <c r="G3" s="3">
+        <v>1</v>
+      </c>
+      <c r="H3" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="I3" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="J3" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="K3" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="D4" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="J4" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="K4" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="L4" s="3">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="3">
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="H5" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="L5" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="M5" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="N5" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1</v>
+      </c>
+      <c r="D7" s="3">
+        <v>2</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0</v>
+      </c>
+      <c r="G7" s="3">
         <v>1.5</v>
       </c>
-      <c r="D6" s="3">
-        <v>1</v>
-      </c>
-      <c r="E6" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="F6" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="G6" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="H6" s="3">
-        <v>-0.5</v>
-      </c>
-      <c r="I6" s="3">
-        <v>1</v>
-      </c>
-      <c r="J6" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="K6" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="L6" s="3">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="3">
+      <c r="H7" s="3">
+        <v>1</v>
+      </c>
+      <c r="I7" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="J7" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="K7" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="L7" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="M7" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="N7" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0</v>
+      </c>
+      <c r="G8" s="3">
         <v>0.75</v>
       </c>
-      <c r="D7" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="E7" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="F7" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="G7" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="H7" s="3">
-        <v>-0.5</v>
-      </c>
-      <c r="I7" s="3">
-        <v>1</v>
-      </c>
-      <c r="J7" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="K7" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="L7" s="3">
+      <c r="H8" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="I8" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="J8" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="K8" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="L8" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="M8" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="N8" s="3">
         <v>0.5</v>
       </c>
     </row>
@@ -885,43 +945,59 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="88.7109375" customWidth="1"/>
-    <col min="3" max="3" width="42.5703125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="15" style="3" customWidth="1"/>
+    <col min="2" max="2" width="144.7109375" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="29.7109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="30.7109375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="38.7109375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="7.7109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="3" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -929,7 +1005,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="3">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D2" s="3">
         <v>1</v>
@@ -938,18 +1014,30 @@
         <v>1</v>
       </c>
       <c r="F2" s="3">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="H3" s="3">
+        <v>1</v>
+      </c>
+      <c r="I3" s="3">
+        <v>1</v>
+      </c>
+      <c r="J3" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -957,29 +1045,20 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="D6" s="3">
-        <v>1</v>
-      </c>
-      <c r="E6" s="3">
-        <v>1</v>
-      </c>
-      <c r="F6" s="3">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C7" s="3">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D7" s="3">
         <v>1</v>
@@ -988,6 +1067,47 @@
         <v>1</v>
       </c>
       <c r="F7" s="3">
+        <v>1</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="H7" s="3">
+        <v>1</v>
+      </c>
+      <c r="I7" s="3">
+        <v>1</v>
+      </c>
+      <c r="J7" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1</v>
+      </c>
+      <c r="E8" s="3">
+        <v>1</v>
+      </c>
+      <c r="F8" s="3">
+        <v>1</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="H8" s="3">
+        <v>1</v>
+      </c>
+      <c r="I8" s="3">
+        <v>1</v>
+      </c>
+      <c r="J8" s="3">
         <v>0.5</v>
       </c>
     </row>
@@ -997,57 +1117,71 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:J6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="88.7109375" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="23.85546875" style="3" customWidth="1"/>
-    <col min="5" max="7" width="27.140625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="20.5703125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="26" style="3" customWidth="1"/>
-    <col min="10" max="10" width="35.85546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="144.7109375" customWidth="1"/>
+    <col min="3" max="3" width="65.7109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="31.7109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="21.7109375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="24.7109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="24.7109375" style="3" customWidth="1"/>
+    <col min="10" max="10" width="24.7109375" style="3" customWidth="1"/>
+    <col min="11" max="11" width="18.7109375" style="3" customWidth="1"/>
+    <col min="12" max="12" width="23.7109375" style="3" customWidth="1"/>
+    <col min="13" max="13" width="32.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1055,39 +1189,48 @@
         <v>6</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1095,32 +1238,49 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C6" s="3">
-        <v>1</v>
-      </c>
-      <c r="D6" s="3">
-        <v>1</v>
-      </c>
-      <c r="E6" s="3">
-        <v>1</v>
-      </c>
-      <c r="F6" s="3">
-        <v>1</v>
-      </c>
-      <c r="G6" s="3">
-        <v>1</v>
-      </c>
-      <c r="H6" s="3">
-        <v>1</v>
-      </c>
-      <c r="I6" s="3">
-        <v>1</v>
-      </c>
-      <c r="J6" s="3">
+    <row r="5" spans="1:13">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1</v>
+      </c>
+      <c r="F7" s="3">
+        <v>1</v>
+      </c>
+      <c r="G7" s="3">
+        <v>1</v>
+      </c>
+      <c r="H7" s="3">
+        <v>1</v>
+      </c>
+      <c r="I7" s="3">
+        <v>1</v>
+      </c>
+      <c r="J7" s="3">
+        <v>1</v>
+      </c>
+      <c r="K7" s="3">
+        <v>1</v>
+      </c>
+      <c r="L7" s="3">
+        <v>1</v>
+      </c>
+      <c r="M7" s="3">
         <v>1</v>
       </c>
     </row>
@@ -1130,47 +1290,55 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:G6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="88.7109375" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="33.7109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="31.5703125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="49.140625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="144.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="30.7109375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="28.7109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="44.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1178,57 +1346,77 @@
         <v>6</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C6" s="3">
-        <v>1</v>
-      </c>
-      <c r="D6" s="3">
-        <v>1</v>
-      </c>
-      <c r="E6" s="3">
-        <v>1</v>
-      </c>
-      <c r="F6" s="3">
-        <v>1</v>
-      </c>
-      <c r="G6" s="3">
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1</v>
+      </c>
+      <c r="F7" s="3">
+        <v>1</v>
+      </c>
+      <c r="G7" s="3">
+        <v>1</v>
+      </c>
+      <c r="H7" s="3">
+        <v>1</v>
+      </c>
+      <c r="I7" s="3">
         <v>2</v>
       </c>
     </row>
@@ -1238,82 +1426,90 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:E6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="88.7109375" customWidth="1"/>
-    <col min="3" max="3" width="28.28515625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="24.85546875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="39.28515625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="144.7109375" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="35.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C3" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C6" s="3">
-        <v>1</v>
-      </c>
-      <c r="D6" s="3">
-        <v>1</v>
-      </c>
-      <c r="E6" s="3">
+      <c r="D4" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1</v>
+      </c>
+      <c r="E7" s="3">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Work for the day ⌛ Another paper review completed
</commit_message>
<xml_diff>
--- a/papers/stats/stats_spreadsheet.xlsx
+++ b/papers/stats/stats_spreadsheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="72">
   <si>
     <t>Paper Title</t>
   </si>
@@ -48,6 +48,9 @@
     <t>Process and Reactive Schizophrenia: Some Conceptions and Issues</t>
   </si>
   <si>
+    <t>Speech Fluency and Schizophrenic Negative Signs</t>
+  </si>
+  <si>
     <t>Thought disorder or speech disorder in schizophrenia?</t>
   </si>
   <si>
@@ -60,6 +63,9 @@
     <t>Garmezy N</t>
   </si>
   <si>
+    <t>Alpert M, Kotsaftis A, Pouget E.</t>
+  </si>
+  <si>
     <t>Chaika E.</t>
   </si>
   <si>
@@ -102,6 +108,9 @@
     <t>Preoccupation with Syntax Rules</t>
   </si>
   <si>
+    <t>Alogia</t>
+  </si>
+  <si>
     <t>Neologization</t>
   </si>
   <si>
@@ -141,13 +150,19 @@
     <t>Unusual Story</t>
   </si>
   <si>
+    <t>Semi-Structured Interview</t>
+  </si>
+  <si>
+    <t>Review of Altered Tapes</t>
+  </si>
+  <si>
     <t>Scale  for  Assessment  of  Thought,  Language, and Communication</t>
   </si>
   <si>
     <t>Mini-Mental  State  examination</t>
   </si>
   <si>
-    <t>DSM-III-R Criterion</t>
+    <t>DSM Criterion</t>
   </si>
   <si>
     <t>Speech Duration</t>
@@ -174,6 +189,15 @@
     <t>Parenthetical Remarks Identified</t>
   </si>
   <si>
+    <t>Schedule for Affective Disorders and Schizophrenia</t>
+  </si>
+  <si>
+    <t>Response Latency</t>
+  </si>
+  <si>
+    <t>Scale for the Assessment of Negative Symptoms</t>
+  </si>
+  <si>
     <t>X</t>
   </si>
   <si>
@@ -199,6 +223,9 @@
   </si>
   <si>
     <t>Difference with other Neurological Disorders</t>
+  </si>
+  <si>
+    <t>Accoustic Imprecision</t>
   </si>
   <si>
     <t>Classifying Schizophrenic</t>
@@ -572,7 +599,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -584,7 +611,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="144.7109375" customWidth="1"/>
-    <col min="3" max="3" width="26.7109375" customWidth="1"/>
+    <col min="3" max="3" width="32.7109375" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" customWidth="1"/>
     <col min="6" max="6" width="19.7109375" customWidth="1"/>
@@ -619,10 +646,10 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E2" s="2">
         <v>44468</v>
@@ -642,10 +669,10 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E3" s="2">
         <v>44460</v>
@@ -665,10 +692,10 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E4" s="2">
         <v>44466</v>
@@ -688,18 +715,41 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E5" s="2">
+        <v>44470</v>
+      </c>
+      <c r="F5" s="2">
+        <v>44471</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="2">
         <v>44466</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F6" s="2">
         <v>44466</v>
       </c>
-      <c r="G5">
+      <c r="G6">
         <v>0</v>
       </c>
     </row>
@@ -710,7 +760,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -731,53 +781,57 @@
     <col min="9" max="9" width="16.7109375" style="3" customWidth="1"/>
     <col min="10" max="10" width="26.7109375" style="3" customWidth="1"/>
     <col min="11" max="11" width="31.7109375" style="3" customWidth="1"/>
-    <col min="12" max="12" width="13.7109375" style="3" customWidth="1"/>
-    <col min="13" max="13" width="10.7109375" style="3" customWidth="1"/>
-    <col min="14" max="14" width="11.7109375" style="3" customWidth="1"/>
+    <col min="12" max="12" width="6.7109375" style="3" customWidth="1"/>
+    <col min="13" max="13" width="13.7109375" style="3" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" style="3" customWidth="1"/>
+    <col min="15" max="15" width="11.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:15">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14">
+        <v>31</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -797,7 +851,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:15">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -826,7 +880,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:15">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -834,79 +888,52 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:15">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="H5" s="3">
-        <v>0.5</v>
+      <c r="C5" s="3">
+        <v>1</v>
       </c>
       <c r="L5" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="M5" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="N5" s="3">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14">
-      <c r="A7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" s="3">
-        <v>1</v>
-      </c>
-      <c r="D7" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="M6" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="N6" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="O6" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="3">
         <v>2</v>
       </c>
-      <c r="E7" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="F7" s="3">
-        <v>0</v>
-      </c>
-      <c r="G7" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="H7" s="3">
-        <v>1</v>
-      </c>
-      <c r="I7" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="J7" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="K7" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="L7" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="M7" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="N7" s="3">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14">
-      <c r="A8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" s="3">
-        <v>1</v>
-      </c>
       <c r="D8" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E8" s="3">
         <v>0.5</v>
@@ -915,27 +942,74 @@
         <v>0</v>
       </c>
       <c r="G8" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="H8" s="3">
+        <v>1</v>
+      </c>
+      <c r="I8" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="J8" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="K8" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="L8" s="3">
+        <v>1</v>
+      </c>
+      <c r="M8" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="N8" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="O8" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0</v>
+      </c>
+      <c r="G9" s="3">
         <v>0.75</v>
       </c>
-      <c r="H8" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="I8" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="J8" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="K8" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="L8" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="M8" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="N8" s="3">
+      <c r="H9" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="I9" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="J9" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="K9" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="L9" s="3">
+        <v>1</v>
+      </c>
+      <c r="M9" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="N9" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="O9" s="3">
         <v>0.5</v>
       </c>
     </row>
@@ -946,7 +1020,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -966,38 +1040,46 @@
     <col min="8" max="8" width="7.7109375" style="3" customWidth="1"/>
     <col min="9" max="9" width="9.7109375" style="3" customWidth="1"/>
     <col min="10" max="10" width="13.7109375" style="3" customWidth="1"/>
+    <col min="11" max="11" width="25.7109375" style="3" customWidth="1"/>
+    <col min="12" max="12" width="23.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:12">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
+        <v>42</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1017,7 +1099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:12">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1037,7 +1119,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:12">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1045,46 +1127,31 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:12">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" s="3">
-        <v>1</v>
-      </c>
-      <c r="D7" s="3">
-        <v>1</v>
-      </c>
-      <c r="E7" s="3">
-        <v>1</v>
-      </c>
-      <c r="F7" s="3">
-        <v>1</v>
-      </c>
-      <c r="G7" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="H7" s="3">
-        <v>1</v>
-      </c>
-      <c r="I7" s="3">
-        <v>1</v>
-      </c>
-      <c r="J7" s="3">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="K5" s="3">
+        <v>1</v>
+      </c>
+      <c r="L5" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C8" s="3">
         <v>1</v>
@@ -1109,6 +1176,47 @@
       </c>
       <c r="J8" s="3">
         <v>0.5</v>
+      </c>
+      <c r="K8" s="3">
+        <v>1</v>
+      </c>
+      <c r="L8" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1</v>
+      </c>
+      <c r="E9" s="3">
+        <v>1</v>
+      </c>
+      <c r="F9" s="3">
+        <v>1</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="H9" s="3">
+        <v>1</v>
+      </c>
+      <c r="I9" s="3">
+        <v>1</v>
+      </c>
+      <c r="J9" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="K9" s="3">
+        <v>1</v>
+      </c>
+      <c r="L9" s="3">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1118,7 +1226,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:P8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -1132,7 +1240,7 @@
     <col min="2" max="2" width="144.7109375" customWidth="1"/>
     <col min="3" max="3" width="65.7109375" style="3" customWidth="1"/>
     <col min="4" max="4" width="31.7109375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="19.7109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" style="3" customWidth="1"/>
     <col min="6" max="6" width="15.7109375" style="3" customWidth="1"/>
     <col min="7" max="7" width="21.7109375" style="3" customWidth="1"/>
     <col min="8" max="8" width="24.7109375" style="3" customWidth="1"/>
@@ -1141,47 +1249,59 @@
     <col min="11" max="11" width="18.7109375" style="3" customWidth="1"/>
     <col min="12" max="12" width="23.7109375" style="3" customWidth="1"/>
     <col min="13" max="13" width="32.7109375" style="3" customWidth="1"/>
+    <col min="14" max="14" width="50.7109375" style="3" customWidth="1"/>
+    <col min="15" max="15" width="16.7109375" style="3" customWidth="1"/>
+    <col min="16" max="16" width="45.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:16">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13">
+        <v>55</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1189,16 +1309,16 @@
         <v>6</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1206,31 +1326,31 @@
         <v>7</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1238,49 +1358,81 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:16">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:13">
-      <c r="A7" t="s">
-        <v>52</v>
-      </c>
-      <c r="C7" s="3">
-        <v>1</v>
-      </c>
-      <c r="D7" s="3">
-        <v>1</v>
-      </c>
-      <c r="E7" s="3">
-        <v>1</v>
-      </c>
-      <c r="F7" s="3">
-        <v>1</v>
-      </c>
-      <c r="G7" s="3">
-        <v>1</v>
-      </c>
-      <c r="H7" s="3">
-        <v>1</v>
-      </c>
-      <c r="I7" s="3">
-        <v>1</v>
-      </c>
-      <c r="J7" s="3">
-        <v>1</v>
-      </c>
-      <c r="K7" s="3">
-        <v>1</v>
-      </c>
-      <c r="L7" s="3">
-        <v>1</v>
-      </c>
-      <c r="M7" s="3">
+      <c r="E5" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1</v>
+      </c>
+      <c r="E8" s="3">
+        <v>2</v>
+      </c>
+      <c r="F8" s="3">
+        <v>1</v>
+      </c>
+      <c r="G8" s="3">
+        <v>1</v>
+      </c>
+      <c r="H8" s="3">
+        <v>2</v>
+      </c>
+      <c r="I8" s="3">
+        <v>1</v>
+      </c>
+      <c r="J8" s="3">
+        <v>1</v>
+      </c>
+      <c r="K8" s="3">
+        <v>1</v>
+      </c>
+      <c r="L8" s="3">
+        <v>1</v>
+      </c>
+      <c r="M8" s="3">
+        <v>1</v>
+      </c>
+      <c r="N8" s="3">
+        <v>1</v>
+      </c>
+      <c r="O8" s="3">
+        <v>1</v>
+      </c>
+      <c r="P8" s="3">
         <v>1</v>
       </c>
     </row>
@@ -1291,7 +1443,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -1310,35 +1462,39 @@
     <col min="7" max="7" width="30.7109375" style="3" customWidth="1"/>
     <col min="8" max="8" width="28.7109375" style="3" customWidth="1"/>
     <col min="9" max="9" width="44.7109375" style="3" customWidth="1"/>
+    <col min="10" max="10" width="21.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+        <v>67</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1346,13 +1502,13 @@
         <v>6</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1360,22 +1516,22 @@
         <v>7</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1383,41 +1539,55 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:10">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" t="s">
-        <v>52</v>
-      </c>
-      <c r="C7" s="3">
-        <v>1</v>
-      </c>
-      <c r="D7" s="3">
-        <v>1</v>
-      </c>
-      <c r="E7" s="3">
-        <v>1</v>
-      </c>
-      <c r="F7" s="3">
-        <v>1</v>
-      </c>
-      <c r="G7" s="3">
-        <v>1</v>
-      </c>
-      <c r="H7" s="3">
-        <v>1</v>
-      </c>
-      <c r="I7" s="3">
+      <c r="J5" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1</v>
+      </c>
+      <c r="E8" s="3">
+        <v>1</v>
+      </c>
+      <c r="F8" s="3">
+        <v>1</v>
+      </c>
+      <c r="G8" s="3">
+        <v>1</v>
+      </c>
+      <c r="H8" s="3">
+        <v>1</v>
+      </c>
+      <c r="I8" s="3">
         <v>2</v>
+      </c>
+      <c r="J8" s="3">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1427,7 +1597,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -1449,13 +1619,13 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1474,7 +1644,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1485,7 +1655,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1495,21 +1665,29 @@
       <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>52</v>
-      </c>
-      <c r="C7" s="3">
-        <v>1</v>
-      </c>
-      <c r="D7" s="3">
-        <v>1</v>
-      </c>
-      <c r="E7" s="3">
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1</v>
+      </c>
+      <c r="E8" s="3">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Another paper processed 📖 Added grammarly to VS code
</commit_message>
<xml_diff>
--- a/papers/stats/stats_spreadsheet.xlsx
+++ b/papers/stats/stats_spreadsheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="76">
   <si>
     <t>Paper Title</t>
   </si>
@@ -48,6 +48,9 @@
     <t>Process and Reactive Schizophrenia: Some Conceptions and Issues</t>
   </si>
   <si>
+    <t>Speech and Language Processing: An Introduction to Natural Language Processing, Computational Linguistics, and Speech Recognition</t>
+  </si>
+  <si>
     <t>Speech Fluency and Schizophrenic Negative Signs</t>
   </si>
   <si>
@@ -63,6 +66,9 @@
     <t>Garmezy N</t>
   </si>
   <si>
+    <t>Martin J</t>
+  </si>
+  <si>
     <t>Alpert M, Kotsaftis A, Pouget E.</t>
   </si>
   <si>
@@ -78,6 +84,9 @@
     <t>Fall 1970</t>
   </si>
   <si>
+    <t>2008</t>
+  </si>
+  <si>
     <t>1982</t>
   </si>
   <si>
@@ -232,6 +241,9 @@
   </si>
   <si>
     <t>Diagnosis by Prognosis</t>
+  </si>
+  <si>
+    <t>Understanding Language</t>
   </si>
   <si>
     <t>Thought Disorder VS Speech Disorder</t>
@@ -599,7 +611,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -646,10 +658,10 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E2" s="2">
         <v>44468</v>
@@ -669,10 +681,10 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E3" s="2">
         <v>44460</v>
@@ -692,10 +704,10 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E4" s="2">
         <v>44466</v>
@@ -715,16 +727,16 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E5" s="2">
-        <v>44470</v>
+        <v>44471</v>
       </c>
       <c r="F5" s="2">
-        <v>44471</v>
+        <v>44472</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -738,18 +750,41 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E6" s="2">
+        <v>44470</v>
+      </c>
+      <c r="F6" s="2">
+        <v>44471</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="2">
         <v>44466</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F7" s="2">
         <v>44466</v>
       </c>
-      <c r="G6">
+      <c r="G7">
         <v>0</v>
       </c>
     </row>
@@ -760,7 +795,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O9"/>
+  <dimension ref="A1:O10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -792,43 +827,43 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -895,12 +930,6 @@
       <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="3">
-        <v>1</v>
-      </c>
-      <c r="L5" s="3">
-        <v>1</v>
-      </c>
     </row>
     <row r="6" spans="1:15">
       <c r="A6" s="1">
@@ -909,75 +938,45 @@
       <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="H6" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="M6" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="N6" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="O6" s="3">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15">
-      <c r="A8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="3">
-        <v>2</v>
-      </c>
-      <c r="D8" s="3">
-        <v>2</v>
-      </c>
-      <c r="E8" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="F8" s="3">
-        <v>0</v>
-      </c>
-      <c r="G8" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="H8" s="3">
-        <v>1</v>
-      </c>
-      <c r="I8" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="J8" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="K8" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="L8" s="3">
-        <v>1</v>
-      </c>
-      <c r="M8" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="N8" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="O8" s="3">
+      <c r="C6" s="3">
+        <v>1</v>
+      </c>
+      <c r="L6" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="H7" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="M7" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="N7" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="O7" s="3">
         <v>0.5</v>
       </c>
     </row>
     <row r="9" spans="1:15">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C9" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D9" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E9" s="3">
         <v>0.5</v>
@@ -986,30 +985,74 @@
         <v>0</v>
       </c>
       <c r="G9" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="H9" s="3">
+        <v>1</v>
+      </c>
+      <c r="I9" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="J9" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="K9" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="L9" s="3">
+        <v>1</v>
+      </c>
+      <c r="M9" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="N9" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="O9" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0</v>
+      </c>
+      <c r="G10" s="3">
         <v>0.75</v>
       </c>
-      <c r="H9" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="I9" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="J9" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="K9" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="L9" s="3">
-        <v>1</v>
-      </c>
-      <c r="M9" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="N9" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="O9" s="3">
+      <c r="H10" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="I10" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="J10" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="K10" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="L10" s="3">
+        <v>1</v>
+      </c>
+      <c r="M10" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="N10" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="O10" s="3">
         <v>0.5</v>
       </c>
     </row>
@@ -1020,7 +1063,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -1049,34 +1092,34 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -1134,12 +1177,6 @@
       <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="K5" s="3">
-        <v>1</v>
-      </c>
-      <c r="L5" s="3">
-        <v>1</v>
-      </c>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="1">
@@ -1148,45 +1185,24 @@
       <c r="B6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="A8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="3">
-        <v>1</v>
-      </c>
-      <c r="D8" s="3">
-        <v>1</v>
-      </c>
-      <c r="E8" s="3">
-        <v>1</v>
-      </c>
-      <c r="F8" s="3">
-        <v>1</v>
-      </c>
-      <c r="G8" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="H8" s="3">
-        <v>1</v>
-      </c>
-      <c r="I8" s="3">
-        <v>1</v>
-      </c>
-      <c r="J8" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="K8" s="3">
-        <v>1</v>
-      </c>
-      <c r="L8" s="3">
-        <v>1</v>
+      <c r="K6" s="3">
+        <v>1</v>
+      </c>
+      <c r="L6" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C9" s="3">
         <v>1</v>
@@ -1216,6 +1232,41 @@
         <v>1</v>
       </c>
       <c r="L9" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1</v>
+      </c>
+      <c r="E10" s="3">
+        <v>1</v>
+      </c>
+      <c r="F10" s="3">
+        <v>1</v>
+      </c>
+      <c r="G10" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="H10" s="3">
+        <v>1</v>
+      </c>
+      <c r="I10" s="3">
+        <v>1</v>
+      </c>
+      <c r="J10" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="K10" s="3">
+        <v>1</v>
+      </c>
+      <c r="L10" s="3">
         <v>1</v>
       </c>
     </row>
@@ -1226,7 +1277,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P8"/>
+  <dimension ref="A1:P9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -1259,46 +1310,46 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:16">
@@ -1309,13 +1360,13 @@
         <v>6</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -1326,28 +1377,28 @@
         <v>7</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -1365,21 +1416,6 @@
       <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="N5" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="O5" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="P5" s="3" t="s">
-        <v>59</v>
-      </c>
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="1">
@@ -1388,51 +1424,74 @@
       <c r="B6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:16">
-      <c r="A8" t="s">
-        <v>60</v>
-      </c>
-      <c r="C8" s="3">
-        <v>1</v>
-      </c>
-      <c r="D8" s="3">
-        <v>1</v>
-      </c>
-      <c r="E8" s="3">
+      <c r="E6" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="A9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1</v>
+      </c>
+      <c r="E9" s="3">
         <v>2</v>
       </c>
-      <c r="F8" s="3">
-        <v>1</v>
-      </c>
-      <c r="G8" s="3">
-        <v>1</v>
-      </c>
-      <c r="H8" s="3">
+      <c r="F9" s="3">
+        <v>1</v>
+      </c>
+      <c r="G9" s="3">
+        <v>1</v>
+      </c>
+      <c r="H9" s="3">
         <v>2</v>
       </c>
-      <c r="I8" s="3">
-        <v>1</v>
-      </c>
-      <c r="J8" s="3">
-        <v>1</v>
-      </c>
-      <c r="K8" s="3">
-        <v>1</v>
-      </c>
-      <c r="L8" s="3">
-        <v>1</v>
-      </c>
-      <c r="M8" s="3">
-        <v>1</v>
-      </c>
-      <c r="N8" s="3">
-        <v>1</v>
-      </c>
-      <c r="O8" s="3">
-        <v>1</v>
-      </c>
-      <c r="P8" s="3">
+      <c r="I9" s="3">
+        <v>1</v>
+      </c>
+      <c r="J9" s="3">
+        <v>1</v>
+      </c>
+      <c r="K9" s="3">
+        <v>1</v>
+      </c>
+      <c r="L9" s="3">
+        <v>1</v>
+      </c>
+      <c r="M9" s="3">
+        <v>1</v>
+      </c>
+      <c r="N9" s="3">
+        <v>1</v>
+      </c>
+      <c r="O9" s="3">
+        <v>1</v>
+      </c>
+      <c r="P9" s="3">
         <v>1</v>
       </c>
     </row>
@@ -1443,7 +1502,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -1470,28 +1529,28 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -1502,10 +1561,10 @@
         <v>6</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1516,19 +1575,19 @@
         <v>7</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -1546,9 +1605,6 @@
       <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="3" t="s">
-        <v>59</v>
-      </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="1">
@@ -1557,36 +1613,47 @@
       <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="I6" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" t="s">
-        <v>60</v>
-      </c>
-      <c r="C8" s="3">
-        <v>1</v>
-      </c>
-      <c r="D8" s="3">
-        <v>1</v>
-      </c>
-      <c r="E8" s="3">
-        <v>1</v>
-      </c>
-      <c r="F8" s="3">
-        <v>1</v>
-      </c>
-      <c r="G8" s="3">
-        <v>1</v>
-      </c>
-      <c r="H8" s="3">
-        <v>1</v>
-      </c>
-      <c r="I8" s="3">
+      <c r="J6" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1</v>
+      </c>
+      <c r="E9" s="3">
+        <v>1</v>
+      </c>
+      <c r="F9" s="3">
+        <v>1</v>
+      </c>
+      <c r="G9" s="3">
+        <v>1</v>
+      </c>
+      <c r="H9" s="3">
+        <v>1</v>
+      </c>
+      <c r="I9" s="3">
         <v>2</v>
       </c>
-      <c r="J8" s="3">
+      <c r="J9" s="3">
         <v>1</v>
       </c>
     </row>
@@ -1597,7 +1664,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -1611,24 +1678,28 @@
     <col min="2" max="2" width="144.7109375" customWidth="1"/>
     <col min="3" max="3" width="25.7109375" style="3" customWidth="1"/>
     <col min="4" max="4" width="22.7109375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="35.7109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="35.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+        <v>74</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1636,7 +1707,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:6">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1644,10 +1715,10 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1655,39 +1726,53 @@
         <v>8</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="E5" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
-        <v>60</v>
-      </c>
-      <c r="C8" s="3">
-        <v>1</v>
-      </c>
-      <c r="D8" s="3">
-        <v>1</v>
-      </c>
-      <c r="E8" s="3">
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1</v>
+      </c>
+      <c r="E9" s="3">
+        <v>1</v>
+      </c>
+      <c r="F9" s="3">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Another paper processed 📖
</commit_message>
<xml_diff>
--- a/papers/stats/stats_spreadsheet.xlsx
+++ b/papers/stats/stats_spreadsheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="86">
   <si>
     <t>Paper Title</t>
   </si>
@@ -42,6 +42,9 @@
     <t>Age-Related Differences in Formal Thought Disorderin Chronically Hospitalized Schizophrenic Patients:A Cross-Sectional Study Across Nine Decades</t>
   </si>
   <si>
+    <t>Attenuated Frontal Activation During a Verbal Fluency Taskin Patients With Schizophrenia</t>
+  </si>
+  <si>
     <t>Psycholinguistic aspects of pauses and temporal patterns in schizophrenic speech</t>
   </si>
   <si>
@@ -60,6 +63,9 @@
     <t>Harvey F, Leibman L, Al E.</t>
   </si>
   <si>
+    <t>Curtis V, Bullmore E, Brammer M, et al.</t>
+  </si>
+  <si>
     <t>Clemmer, Edward J.</t>
   </si>
   <si>
@@ -78,6 +84,9 @@
     <t>1997</t>
   </si>
   <si>
+    <t>1998</t>
+  </si>
+  <si>
     <t>1980</t>
   </si>
   <si>
@@ -102,6 +111,12 @@
     <t>Absence of Self Monitoring</t>
   </si>
   <si>
+    <t>Cerebral Frontal Region Attenuated</t>
+  </si>
+  <si>
+    <t>Medial Parietal Cortex Strengthen</t>
+  </si>
+  <si>
     <t>Gibberish</t>
   </si>
   <si>
@@ -147,6 +162,12 @@
     <t>Open Interview with Caregivers</t>
   </si>
   <si>
+    <t>Magnetic Resonance Imaging</t>
+  </si>
+  <si>
+    <t>Positron Emission Tomography</t>
+  </si>
+  <si>
     <t>Matching of Control with Schizophrenic</t>
   </si>
   <si>
@@ -174,6 +195,18 @@
     <t>DSM Criterion</t>
   </si>
   <si>
+    <t>Cerabral Blood Flow</t>
+  </si>
+  <si>
+    <t>Schedule for Affective Disorders and Schizophrenia</t>
+  </si>
+  <si>
+    <t>Scale for the Assessment of Positive Symptoms</t>
+  </si>
+  <si>
+    <t>Scale for the Assessment of Negative Symptoms</t>
+  </si>
+  <si>
     <t>Speech Duration</t>
   </si>
   <si>
@@ -198,15 +231,9 @@
     <t>Parenthetical Remarks Identified</t>
   </si>
   <si>
-    <t>Schedule for Affective Disorders and Schizophrenia</t>
-  </si>
-  <si>
     <t>Response Latency</t>
   </si>
   <si>
-    <t>Scale for the Assessment of Negative Symptoms</t>
-  </si>
-  <si>
     <t>X</t>
   </si>
   <si>
@@ -219,13 +246,16 @@
     <t>Different Environments</t>
   </si>
   <si>
+    <t>Small Sample</t>
+  </si>
+  <si>
+    <t>MRI Account for Perturbances</t>
+  </si>
+  <si>
+    <t>Schizophrenic under Medication</t>
+  </si>
+  <si>
     <t>Restrictive Sample</t>
-  </si>
-  <si>
-    <t>Small Sample</t>
-  </si>
-  <si>
-    <t>Schizophrenic under Medication</t>
   </si>
   <si>
     <t>Schizophrenic under Lobotomy</t>
@@ -611,7 +641,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -623,7 +653,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="144.7109375" customWidth="1"/>
-    <col min="3" max="3" width="32.7109375" customWidth="1"/>
+    <col min="3" max="3" width="39.7109375" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" customWidth="1"/>
     <col min="6" max="6" width="19.7109375" customWidth="1"/>
@@ -658,10 +688,10 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E2" s="2">
         <v>44468</v>
@@ -681,19 +711,19 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E3" s="2">
-        <v>44460</v>
+        <v>44472</v>
       </c>
       <c r="F3" s="2">
-        <v>44462</v>
+        <v>44473</v>
       </c>
       <c r="G3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -704,19 +734,19 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E4" s="2">
-        <v>44466</v>
+        <v>44460</v>
       </c>
       <c r="F4" s="2">
-        <v>2958465</v>
+        <v>44462</v>
       </c>
       <c r="G4">
-        <v>2913999</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -727,19 +757,19 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E5" s="2">
-        <v>44471</v>
+        <v>44466</v>
       </c>
       <c r="F5" s="2">
-        <v>44472</v>
+        <v>2958465</v>
       </c>
       <c r="G5">
-        <v>1</v>
+        <v>2913999</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -750,16 +780,16 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="E6" s="2">
-        <v>44470</v>
+        <v>44471</v>
       </c>
       <c r="F6" s="2">
-        <v>44471</v>
+        <v>44472</v>
       </c>
       <c r="G6">
         <v>1</v>
@@ -773,18 +803,41 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E7" s="2">
+        <v>44470</v>
+      </c>
+      <c r="F7" s="2">
+        <v>44471</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="2">
         <v>44466</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F8" s="2">
         <v>44466</v>
       </c>
-      <c r="G7">
+      <c r="G8">
         <v>0</v>
       </c>
     </row>
@@ -795,7 +848,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O10"/>
+  <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -811,62 +864,70 @@
     <col min="4" max="4" width="27.7109375" style="3" customWidth="1"/>
     <col min="5" max="5" width="15.7109375" style="3" customWidth="1"/>
     <col min="6" max="6" width="26.7109375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" style="3" customWidth="1"/>
-    <col min="9" max="9" width="16.7109375" style="3" customWidth="1"/>
-    <col min="10" max="10" width="26.7109375" style="3" customWidth="1"/>
-    <col min="11" max="11" width="31.7109375" style="3" customWidth="1"/>
-    <col min="12" max="12" width="6.7109375" style="3" customWidth="1"/>
-    <col min="13" max="13" width="13.7109375" style="3" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" style="3" customWidth="1"/>
-    <col min="15" max="15" width="11.7109375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="34.7109375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="33.7109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="3" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" style="3" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" style="3" customWidth="1"/>
+    <col min="12" max="12" width="26.7109375" style="3" customWidth="1"/>
+    <col min="13" max="13" width="31.7109375" style="3" customWidth="1"/>
+    <col min="14" max="14" width="6.7109375" style="3" customWidth="1"/>
+    <col min="15" max="15" width="13.7109375" style="3" customWidth="1"/>
+    <col min="16" max="16" width="10.7109375" style="3" customWidth="1"/>
+    <col min="17" max="17" width="11.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:17">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15">
+        <v>38</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -886,44 +947,50 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:17">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="3">
-        <v>1</v>
-      </c>
-      <c r="F3" s="3">
-        <v>-0.5</v>
-      </c>
       <c r="G3" s="3">
         <v>1</v>
       </c>
       <c r="H3" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="I3" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="J3" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="K3" s="3">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:15">
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3">
+        <v>-0.5</v>
+      </c>
+      <c r="I4" s="3">
+        <v>1</v>
+      </c>
+      <c r="J4" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="K4" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="L4" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="M4" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -931,96 +998,60 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:17">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="3">
-        <v>1</v>
-      </c>
-      <c r="L6" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15">
+    </row>
+    <row r="7" spans="1:17">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="H7" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="M7" s="3">
-        <v>0.5</v>
+      <c r="C7" s="3">
+        <v>1</v>
       </c>
       <c r="N7" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="O7" s="3">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15">
-      <c r="A9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="J8" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="O8" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="P8" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
+      <c r="A10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="3">
         <v>2</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D10" s="3">
         <v>2</v>
-      </c>
-      <c r="E9" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="F9" s="3">
-        <v>0</v>
-      </c>
-      <c r="G9" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="H9" s="3">
-        <v>1</v>
-      </c>
-      <c r="I9" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="J9" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="K9" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="L9" s="3">
-        <v>1</v>
-      </c>
-      <c r="M9" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="N9" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="O9" s="3">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15">
-      <c r="A10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" s="3">
-        <v>1</v>
-      </c>
-      <c r="D10" s="3">
-        <v>1</v>
       </c>
       <c r="E10" s="3">
         <v>0.5</v>
@@ -1029,30 +1060,86 @@
         <v>0</v>
       </c>
       <c r="G10" s="3">
+        <v>1</v>
+      </c>
+      <c r="H10" s="3">
+        <v>1</v>
+      </c>
+      <c r="I10" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="J10" s="3">
+        <v>1</v>
+      </c>
+      <c r="K10" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="L10" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="M10" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="N10" s="3">
+        <v>1</v>
+      </c>
+      <c r="O10" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="P10" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="Q10" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
+      <c r="A11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="3">
+        <v>1</v>
+      </c>
+      <c r="D11" s="3">
+        <v>1</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0</v>
+      </c>
+      <c r="G11" s="3">
+        <v>1</v>
+      </c>
+      <c r="H11" s="3">
+        <v>1</v>
+      </c>
+      <c r="I11" s="3">
         <v>0.75</v>
       </c>
-      <c r="H10" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="I10" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="J10" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="K10" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="L10" s="3">
-        <v>1</v>
-      </c>
-      <c r="M10" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="N10" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="O10" s="3">
+      <c r="J11" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="K11" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="L11" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="M11" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="N11" s="3">
+        <v>1</v>
+      </c>
+      <c r="O11" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="P11" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="Q11" s="3">
         <v>0.5</v>
       </c>
     </row>
@@ -1063,7 +1150,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -1079,50 +1166,58 @@
     <col min="4" max="4" width="29.7109375" style="3" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" style="3" customWidth="1"/>
     <col min="6" max="6" width="30.7109375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="38.7109375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="7.7109375" style="3" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" style="3" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" style="3" customWidth="1"/>
-    <col min="11" max="11" width="25.7109375" style="3" customWidth="1"/>
-    <col min="12" max="12" width="23.7109375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="26.7109375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="28.7109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="38.7109375" style="3" customWidth="1"/>
+    <col min="10" max="10" width="7.7109375" style="3" customWidth="1"/>
+    <col min="11" max="11" width="9.7109375" style="3" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" style="3" customWidth="1"/>
+    <col min="13" max="13" width="25.7109375" style="3" customWidth="1"/>
+    <col min="14" max="14" width="23.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:14">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12">
+        <v>52</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1142,7 +1237,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:14">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1150,27 +1245,36 @@
         <v>7</v>
       </c>
       <c r="G3" s="3">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="H3" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I3" s="3">
         <v>1</v>
       </c>
-      <c r="J3" s="3">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:12">
+      <c r="I4" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="J4" s="3">
+        <v>1</v>
+      </c>
+      <c r="K4" s="3">
+        <v>1</v>
+      </c>
+      <c r="L4" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1178,66 +1282,39 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:14">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="K6" s="3">
-        <v>1</v>
-      </c>
-      <c r="L6" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:12">
-      <c r="A9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" s="3">
-        <v>1</v>
-      </c>
-      <c r="D9" s="3">
-        <v>1</v>
-      </c>
-      <c r="E9" s="3">
-        <v>1</v>
-      </c>
-      <c r="F9" s="3">
-        <v>1</v>
-      </c>
-      <c r="G9" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="H9" s="3">
-        <v>1</v>
-      </c>
-      <c r="I9" s="3">
-        <v>1</v>
-      </c>
-      <c r="J9" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="K9" s="3">
-        <v>1</v>
-      </c>
-      <c r="L9" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
+      <c r="M7" s="3">
+        <v>1</v>
+      </c>
+      <c r="N7" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C10" s="3">
         <v>1</v>
@@ -1252,21 +1329,68 @@
         <v>1</v>
       </c>
       <c r="G10" s="3">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="H10" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I10" s="3">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="J10" s="3">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="K10" s="3">
         <v>1</v>
       </c>
       <c r="L10" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="M10" s="3">
+        <v>1</v>
+      </c>
+      <c r="N10" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="3">
+        <v>1</v>
+      </c>
+      <c r="D11" s="3">
+        <v>1</v>
+      </c>
+      <c r="E11" s="3">
+        <v>1</v>
+      </c>
+      <c r="F11" s="3">
+        <v>1</v>
+      </c>
+      <c r="G11" s="3">
+        <v>1</v>
+      </c>
+      <c r="H11" s="3">
+        <v>0</v>
+      </c>
+      <c r="I11" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="J11" s="3">
+        <v>1</v>
+      </c>
+      <c r="K11" s="3">
+        <v>1</v>
+      </c>
+      <c r="L11" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="M11" s="3">
+        <v>1</v>
+      </c>
+      <c r="N11" s="3">
         <v>1</v>
       </c>
     </row>
@@ -1277,7 +1401,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P9"/>
+  <dimension ref="A1:R10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -1292,67 +1416,75 @@
     <col min="3" max="3" width="65.7109375" style="3" customWidth="1"/>
     <col min="4" max="4" width="31.7109375" style="3" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="21.7109375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="24.7109375" style="3" customWidth="1"/>
-    <col min="9" max="9" width="24.7109375" style="3" customWidth="1"/>
-    <col min="10" max="10" width="24.7109375" style="3" customWidth="1"/>
-    <col min="11" max="11" width="18.7109375" style="3" customWidth="1"/>
-    <col min="12" max="12" width="23.7109375" style="3" customWidth="1"/>
-    <col min="13" max="13" width="32.7109375" style="3" customWidth="1"/>
-    <col min="14" max="14" width="50.7109375" style="3" customWidth="1"/>
-    <col min="15" max="15" width="16.7109375" style="3" customWidth="1"/>
-    <col min="16" max="16" width="45.7109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="50.7109375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="45.7109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="45.7109375" style="3" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" style="3" customWidth="1"/>
+    <col min="11" max="11" width="21.7109375" style="3" customWidth="1"/>
+    <col min="12" max="12" width="24.7109375" style="3" customWidth="1"/>
+    <col min="13" max="13" width="24.7109375" style="3" customWidth="1"/>
+    <col min="14" max="14" width="24.7109375" style="3" customWidth="1"/>
+    <col min="15" max="15" width="18.7109375" style="3" customWidth="1"/>
+    <col min="16" max="16" width="23.7109375" style="3" customWidth="1"/>
+    <col min="17" max="17" width="32.7109375" style="3" customWidth="1"/>
+    <col min="18" max="18" width="16.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:18">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16">
+        <v>68</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1360,56 +1492,74 @@
         <v>6</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
+      <c r="C3" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="F3" s="3" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:16">
+      <c r="J4" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1417,81 +1567,95 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:18">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="N6" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="O6" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="P6" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16">
+    </row>
+    <row r="7" spans="1:18">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:16">
-      <c r="A9" t="s">
-        <v>63</v>
-      </c>
-      <c r="C9" s="3">
-        <v>1</v>
-      </c>
-      <c r="D9" s="3">
-        <v>1</v>
-      </c>
-      <c r="E9" s="3">
+      <c r="E7" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="R7" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
+      <c r="A10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" s="3">
         <v>2</v>
       </c>
-      <c r="F9" s="3">
-        <v>1</v>
-      </c>
-      <c r="G9" s="3">
-        <v>1</v>
-      </c>
-      <c r="H9" s="3">
+      <c r="D10" s="3">
+        <v>1</v>
+      </c>
+      <c r="E10" s="3">
+        <v>3</v>
+      </c>
+      <c r="F10" s="3">
+        <v>1</v>
+      </c>
+      <c r="G10" s="3">
         <v>2</v>
       </c>
-      <c r="I9" s="3">
-        <v>1</v>
-      </c>
-      <c r="J9" s="3">
-        <v>1</v>
-      </c>
-      <c r="K9" s="3">
-        <v>1</v>
-      </c>
-      <c r="L9" s="3">
-        <v>1</v>
-      </c>
-      <c r="M9" s="3">
-        <v>1</v>
-      </c>
-      <c r="N9" s="3">
-        <v>1</v>
-      </c>
-      <c r="O9" s="3">
-        <v>1</v>
-      </c>
-      <c r="P9" s="3">
+      <c r="H10" s="3">
+        <v>1</v>
+      </c>
+      <c r="I10" s="3">
+        <v>2</v>
+      </c>
+      <c r="J10" s="3">
+        <v>1</v>
+      </c>
+      <c r="K10" s="3">
+        <v>1</v>
+      </c>
+      <c r="L10" s="3">
+        <v>2</v>
+      </c>
+      <c r="M10" s="3">
+        <v>1</v>
+      </c>
+      <c r="N10" s="3">
+        <v>1</v>
+      </c>
+      <c r="O10" s="3">
+        <v>1</v>
+      </c>
+      <c r="P10" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="3">
+        <v>1</v>
+      </c>
+      <c r="R10" s="3">
         <v>1</v>
       </c>
     </row>
@@ -1502,7 +1666,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -1516,44 +1680,48 @@
     <col min="2" max="2" width="144.7109375" customWidth="1"/>
     <col min="3" max="3" width="16.7109375" style="3" customWidth="1"/>
     <col min="4" max="4" width="22.7109375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="28.7109375" style="3" customWidth="1"/>
     <col min="7" max="7" width="30.7109375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="28.7109375" style="3" customWidth="1"/>
-    <col min="9" max="9" width="44.7109375" style="3" customWidth="1"/>
-    <col min="10" max="10" width="21.7109375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="18.7109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="28.7109375" style="3" customWidth="1"/>
+    <col min="10" max="10" width="44.7109375" style="3" customWidth="1"/>
+    <col min="11" max="11" width="21.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
+        <v>80</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1561,13 +1729,13 @@
         <v>6</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1575,30 +1743,39 @@
         <v>7</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="E4" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1606,54 +1783,65 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:11">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="J6" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" t="s">
-        <v>63</v>
-      </c>
-      <c r="C9" s="3">
-        <v>1</v>
-      </c>
-      <c r="D9" s="3">
-        <v>1</v>
-      </c>
-      <c r="E9" s="3">
-        <v>1</v>
-      </c>
-      <c r="F9" s="3">
-        <v>1</v>
-      </c>
-      <c r="G9" s="3">
-        <v>1</v>
-      </c>
-      <c r="H9" s="3">
-        <v>1</v>
-      </c>
-      <c r="I9" s="3">
+      <c r="K7" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1</v>
+      </c>
+      <c r="E10" s="3">
         <v>2</v>
       </c>
-      <c r="J9" s="3">
+      <c r="F10" s="3">
+        <v>1</v>
+      </c>
+      <c r="G10" s="3">
+        <v>2</v>
+      </c>
+      <c r="H10" s="3">
+        <v>1</v>
+      </c>
+      <c r="I10" s="3">
+        <v>1</v>
+      </c>
+      <c r="J10" s="3">
+        <v>2</v>
+      </c>
+      <c r="K10" s="3">
         <v>1</v>
       </c>
     </row>
@@ -1664,7 +1852,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -1687,16 +1875,16 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -1714,9 +1902,6 @@
       <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>62</v>
-      </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1">
@@ -1725,8 +1910,8 @@
       <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>62</v>
+      <c r="C4" s="3" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1736,8 +1921,8 @@
       <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>62</v>
+      <c r="D5" s="3" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1747,6 +1932,9 @@
       <c r="B6" t="s">
         <v>10</v>
       </c>
+      <c r="E6" s="3" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1">
@@ -1755,24 +1943,32 @@
       <c r="B7" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" t="s">
-        <v>63</v>
-      </c>
-      <c r="C9" s="3">
-        <v>1</v>
-      </c>
-      <c r="D9" s="3">
-        <v>1</v>
-      </c>
-      <c r="E9" s="3">
-        <v>1</v>
-      </c>
-      <c r="F9" s="3">
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1</v>
+      </c>
+      <c r="E10" s="3">
+        <v>1</v>
+      </c>
+      <c r="F10" s="3">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Another paper processed 📖 Script for creating spreadsheet now sorts by start and end date
</commit_message>
<xml_diff>
--- a/papers/stats/stats_spreadsheet.xlsx
+++ b/papers/stats/stats_spreadsheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="154">
   <si>
     <t>Paper Title</t>
   </si>
@@ -42,12 +42,12 @@
     <t>Psycholinguistic aspects of pauses and temporal patterns in schizophrenic speech</t>
   </si>
   <si>
+    <t>Thought disorder or speech disorder in schizophrenia?</t>
+  </si>
+  <si>
     <t>Process and Reactive Schizophrenia: Some Conceptions and Issues</t>
   </si>
   <si>
-    <t>Thought disorder or speech disorder in schizophrenia?</t>
-  </si>
-  <si>
     <t>Age-Related Differences in Formal Thought Disorderin Chronically Hospitalized Schizophrenic Patients:A Cross-Sectional Study Across Nine Decades</t>
   </si>
   <si>
@@ -78,15 +78,18 @@
     <t>Phonetic measures of reduced tongue movement correlate with negative symptom severity in hospitalized patients with first-episode schizophrenia-spectrum disorders</t>
   </si>
   <si>
+    <t>Making a distinction between schizophrenia and bipolar disorder based on temporal parameters in spontaneous speech</t>
+  </si>
+  <si>
     <t>Clemmer, Edward J.</t>
   </si>
   <si>
+    <t>Chaika E.</t>
+  </si>
+  <si>
     <t>Garmezy N</t>
   </si>
   <si>
-    <t>Chaika E.</t>
-  </si>
-  <si>
     <t>Harvey F, Leibman L, Al E.</t>
   </si>
   <si>
@@ -117,15 +120,18 @@
     <t>Covington M. Lunden S. Cristofaro S. et al.</t>
   </si>
   <si>
+    <t>Gosztolya G. Bagi A. Szalóki S et al.</t>
+  </si>
+  <si>
     <t>1980</t>
   </si>
   <si>
+    <t>1982</t>
+  </si>
+  <si>
     <t>Fall 1970</t>
   </si>
   <si>
-    <t>1982</t>
-  </si>
-  <si>
     <t>1997</t>
   </si>
   <si>
@@ -147,6 +153,9 @@
     <t>2012</t>
   </si>
   <si>
+    <t>2020</t>
+  </si>
+  <si>
     <t>Gibberish</t>
   </si>
   <si>
@@ -282,6 +291,12 @@
     <t>Spectral Decomposition</t>
   </si>
   <si>
+    <t>Memory Task</t>
+  </si>
+  <si>
+    <t>Structured Interview</t>
+  </si>
+  <si>
     <t>Speech Duration</t>
   </si>
   <si>
@@ -396,6 +411,15 @@
     <t>F2 Formant</t>
   </si>
   <si>
+    <t>Articulation Rate</t>
+  </si>
+  <si>
+    <t>Speech Tempo</t>
+  </si>
+  <si>
+    <t>Duration of Utterance</t>
+  </si>
+  <si>
     <t>X</t>
   </si>
   <si>
@@ -438,10 +462,10 @@
     <t>Classifying Schizophrenic</t>
   </si>
   <si>
+    <t>Thought Disorder VS Speech Disorder</t>
+  </si>
+  <si>
     <t>Diagnosis by Prognosis</t>
-  </si>
-  <si>
-    <t>Thought Disorder VS Speech Disorder</t>
   </si>
   <si>
     <t>Understanding Language</t>
@@ -821,7 +845,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -868,10 +892,10 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E2" s="2">
         <v>44460</v>
@@ -891,19 +915,19 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E3" s="2">
         <v>44466</v>
       </c>
       <c r="F3" s="2">
-        <v>2958465</v>
+        <v>44466</v>
       </c>
       <c r="G3">
-        <v>2913999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -914,19 +938,19 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E4" s="2">
         <v>44466</v>
       </c>
       <c r="F4" s="2">
-        <v>44466</v>
+        <v>2958465</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>2913999</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -937,10 +961,10 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E5" s="2">
         <v>44468</v>
@@ -960,10 +984,10 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D6" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E6" s="2">
         <v>44470</v>
@@ -983,10 +1007,10 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E7" s="2">
         <v>44471</v>
@@ -1006,10 +1030,10 @@
         <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D8" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E8" s="2">
         <v>44472</v>
@@ -1029,10 +1053,10 @@
         <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D9" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E9" s="2">
         <v>44473</v>
@@ -1052,10 +1076,10 @@
         <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D10" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E10" s="2">
         <v>44475</v>
@@ -1075,10 +1099,10 @@
         <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E11" s="2">
         <v>44477</v>
@@ -1098,10 +1122,10 @@
         <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D12" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E12" s="2">
         <v>44480</v>
@@ -1121,10 +1145,10 @@
         <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D13" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E13" s="2">
         <v>44483</v>
@@ -1144,10 +1168,10 @@
         <v>18</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D14" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E14" s="2">
         <v>44488</v>
@@ -1157,6 +1181,29 @@
       </c>
       <c r="G14">
         <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" s="2">
+        <v>44488</v>
+      </c>
+      <c r="F15" s="2">
+        <v>44489</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1166,7 +1213,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T17"/>
+  <dimension ref="A1:T18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -1203,58 +1250,58 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:20">
@@ -1293,6 +1340,21 @@
       <c r="B3" t="s">
         <v>7</v>
       </c>
+      <c r="C3" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="J3" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="K3" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="L3" s="3">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="4" spans="1:20">
       <c r="A4" s="1">
@@ -1301,21 +1363,6 @@
       <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="D4" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="J4" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="K4" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="L4" s="3">
-        <v>0.5</v>
-      </c>
     </row>
     <row r="5" spans="1:20">
       <c r="A5" s="1">
@@ -1454,89 +1501,44 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:20">
-      <c r="A16" t="s">
-        <v>60</v>
-      </c>
-      <c r="C16" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="D16" s="3">
-        <v>1</v>
-      </c>
-      <c r="E16" s="3">
+    <row r="15" spans="1:20">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="O15" s="3">
         <v>0.5</v>
       </c>
-      <c r="F16" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="G16" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="H16" s="3">
-        <v>1</v>
-      </c>
-      <c r="I16" s="3">
-        <v>2</v>
-      </c>
-      <c r="J16" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="K16" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="L16" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="M16" s="3">
-        <v>4</v>
-      </c>
-      <c r="N16" s="3">
-        <v>2</v>
-      </c>
-      <c r="O16" s="3">
-        <v>1</v>
-      </c>
-      <c r="P16" s="3">
-        <v>1</v>
-      </c>
-      <c r="Q16" s="3">
-        <v>2</v>
-      </c>
-      <c r="R16" s="3">
-        <v>1</v>
-      </c>
-      <c r="S16" s="3">
-        <v>1</v>
-      </c>
-      <c r="T16" s="3">
+      <c r="T15" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:20">
       <c r="A17" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C17" s="3">
-        <v>0.75</v>
+        <v>1.5</v>
       </c>
       <c r="D17" s="3">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E17" s="3">
         <v>0.5</v>
       </c>
       <c r="F17" s="3">
-        <v>0.75</v>
+        <v>1.5</v>
       </c>
       <c r="G17" s="3">
         <v>0.5</v>
       </c>
       <c r="H17" s="3">
-        <v>0.3333333333333333</v>
+        <v>1</v>
       </c>
       <c r="I17" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J17" s="3">
         <v>0.5</v>
@@ -1548,27 +1550,86 @@
         <v>0.5</v>
       </c>
       <c r="M17" s="3">
+        <v>4</v>
+      </c>
+      <c r="N17" s="3">
+        <v>2</v>
+      </c>
+      <c r="O17" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="P17" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="3">
+        <v>2</v>
+      </c>
+      <c r="R17" s="3">
+        <v>1</v>
+      </c>
+      <c r="S17" s="3">
+        <v>1</v>
+      </c>
+      <c r="T17" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20">
+      <c r="A18" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="E18" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="F18" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="G18" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="H18" s="3">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="I18" s="3">
+        <v>1</v>
+      </c>
+      <c r="J18" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="K18" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="L18" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="M18" s="3">
         <v>0.8</v>
       </c>
-      <c r="N17" s="3">
+      <c r="N18" s="3">
         <v>0.6666666666666666</v>
       </c>
-      <c r="O17" s="3">
-        <v>1</v>
-      </c>
-      <c r="P17" s="3">
-        <v>1</v>
-      </c>
-      <c r="Q17" s="3">
-        <v>1</v>
-      </c>
-      <c r="R17" s="3">
-        <v>1</v>
-      </c>
-      <c r="S17" s="3">
-        <v>1</v>
-      </c>
-      <c r="T17" s="3">
+      <c r="O18" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="P18" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="3">
+        <v>1</v>
+      </c>
+      <c r="R18" s="3">
+        <v>1</v>
+      </c>
+      <c r="S18" s="3">
+        <v>1</v>
+      </c>
+      <c r="T18" s="3">
         <v>1</v>
       </c>
     </row>
@@ -1579,7 +1640,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AA17"/>
+  <dimension ref="A1:AC18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -1616,89 +1677,97 @@
     <col min="25" max="25" width="16.7109375" style="3" customWidth="1"/>
     <col min="26" max="26" width="21.7109375" style="3" customWidth="1"/>
     <col min="27" max="27" width="22.7109375" style="3" customWidth="1"/>
+    <col min="28" max="28" width="11.7109375" style="3" customWidth="1"/>
+    <col min="29" max="29" width="20.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27">
+    <row r="1" spans="1:29">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="2" spans="1:27">
+        <v>89</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1718,7 +1787,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:27">
+    <row r="3" spans="1:29">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1726,7 +1795,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:27">
+    <row r="4" spans="1:29">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1734,7 +1803,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:27">
+    <row r="5" spans="1:29">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1754,7 +1823,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:27">
+    <row r="6" spans="1:29">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1768,7 +1837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:27">
+    <row r="7" spans="1:29">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1776,7 +1845,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:27">
+    <row r="8" spans="1:29">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1796,7 +1865,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:27">
+    <row r="9" spans="1:29">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1807,7 +1876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:27">
+    <row r="10" spans="1:29">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1824,7 +1893,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:27">
+    <row r="11" spans="1:29">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1850,7 +1919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:27">
+    <row r="12" spans="1:29">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1873,7 +1942,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:27">
+    <row r="13" spans="1:29">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1893,7 +1962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:27">
+    <row r="14" spans="1:29">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1904,98 +1973,32 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:27">
-      <c r="A16" t="s">
-        <v>60</v>
-      </c>
-      <c r="C16" s="3">
+    <row r="15" spans="1:29">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB15" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC15" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:29">
+      <c r="A17" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" s="3">
         <v>1.5</v>
       </c>
-      <c r="D16" s="3">
-        <v>1</v>
-      </c>
-      <c r="E16" s="3">
+      <c r="D17" s="3">
+        <v>1</v>
+      </c>
+      <c r="E17" s="3">
         <v>2</v>
-      </c>
-      <c r="F16" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="G16" s="3">
-        <v>1</v>
-      </c>
-      <c r="H16" s="3">
-        <v>1</v>
-      </c>
-      <c r="I16" s="3">
-        <v>1</v>
-      </c>
-      <c r="J16" s="3">
-        <v>1</v>
-      </c>
-      <c r="K16" s="3">
-        <v>1</v>
-      </c>
-      <c r="L16" s="3">
-        <v>1</v>
-      </c>
-      <c r="M16" s="3">
-        <v>1</v>
-      </c>
-      <c r="N16" s="3">
-        <v>0</v>
-      </c>
-      <c r="O16" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="P16" s="3">
-        <v>3</v>
-      </c>
-      <c r="Q16" s="3">
-        <v>1</v>
-      </c>
-      <c r="R16" s="3">
-        <v>1</v>
-      </c>
-      <c r="S16" s="3">
-        <v>3</v>
-      </c>
-      <c r="T16" s="3">
-        <v>2</v>
-      </c>
-      <c r="U16" s="3">
-        <v>1</v>
-      </c>
-      <c r="V16" s="3">
-        <v>1</v>
-      </c>
-      <c r="W16" s="3">
-        <v>2</v>
-      </c>
-      <c r="X16" s="3">
-        <v>1</v>
-      </c>
-      <c r="Y16" s="3">
-        <v>1</v>
-      </c>
-      <c r="Z16" s="3">
-        <v>1</v>
-      </c>
-      <c r="AA16" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:27">
-      <c r="A17" t="s">
-        <v>61</v>
-      </c>
-      <c r="C17" s="3">
-        <v>0.75</v>
-      </c>
-      <c r="D17" s="3">
-        <v>1</v>
-      </c>
-      <c r="E17" s="3">
-        <v>1</v>
       </c>
       <c r="F17" s="3">
         <v>0.5</v>
@@ -2025,42 +2028,134 @@
         <v>0</v>
       </c>
       <c r="O17" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="P17" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q17" s="3">
+        <v>1</v>
+      </c>
+      <c r="R17" s="3">
+        <v>1</v>
+      </c>
+      <c r="S17" s="3">
+        <v>3</v>
+      </c>
+      <c r="T17" s="3">
+        <v>2</v>
+      </c>
+      <c r="U17" s="3">
+        <v>1</v>
+      </c>
+      <c r="V17" s="3">
+        <v>1</v>
+      </c>
+      <c r="W17" s="3">
+        <v>2</v>
+      </c>
+      <c r="X17" s="3">
+        <v>1</v>
+      </c>
+      <c r="Y17" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z17" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA17" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB17" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC17" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29">
+      <c r="A18" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" s="3">
         <v>0.75</v>
       </c>
-      <c r="P17" s="3">
-        <v>1</v>
-      </c>
-      <c r="Q17" s="3">
-        <v>1</v>
-      </c>
-      <c r="R17" s="3">
-        <v>1</v>
-      </c>
-      <c r="S17" s="3">
-        <v>1</v>
-      </c>
-      <c r="T17" s="3">
-        <v>1</v>
-      </c>
-      <c r="U17" s="3">
-        <v>1</v>
-      </c>
-      <c r="V17" s="3">
-        <v>1</v>
-      </c>
-      <c r="W17" s="3">
-        <v>1</v>
-      </c>
-      <c r="X17" s="3">
-        <v>1</v>
-      </c>
-      <c r="Y17" s="3">
-        <v>1</v>
-      </c>
-      <c r="Z17" s="3">
-        <v>1</v>
-      </c>
-      <c r="AA17" s="3">
+      <c r="D18" s="3">
+        <v>1</v>
+      </c>
+      <c r="E18" s="3">
+        <v>1</v>
+      </c>
+      <c r="F18" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G18" s="3">
+        <v>1</v>
+      </c>
+      <c r="H18" s="3">
+        <v>1</v>
+      </c>
+      <c r="I18" s="3">
+        <v>1</v>
+      </c>
+      <c r="J18" s="3">
+        <v>1</v>
+      </c>
+      <c r="K18" s="3">
+        <v>1</v>
+      </c>
+      <c r="L18" s="3">
+        <v>1</v>
+      </c>
+      <c r="M18" s="3">
+        <v>1</v>
+      </c>
+      <c r="N18" s="3">
+        <v>0</v>
+      </c>
+      <c r="O18" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="P18" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="3">
+        <v>1</v>
+      </c>
+      <c r="R18" s="3">
+        <v>1</v>
+      </c>
+      <c r="S18" s="3">
+        <v>1</v>
+      </c>
+      <c r="T18" s="3">
+        <v>1</v>
+      </c>
+      <c r="U18" s="3">
+        <v>1</v>
+      </c>
+      <c r="V18" s="3">
+        <v>1</v>
+      </c>
+      <c r="W18" s="3">
+        <v>1</v>
+      </c>
+      <c r="X18" s="3">
+        <v>1</v>
+      </c>
+      <c r="Y18" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z18" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA18" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB18" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC18" s="3">
         <v>1</v>
       </c>
     </row>
@@ -2071,7 +2166,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AN16"/>
+  <dimension ref="A1:AQ17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -2121,128 +2216,140 @@
     <col min="38" max="38" width="36.7109375" style="3" customWidth="1"/>
     <col min="39" max="39" width="10.7109375" style="3" customWidth="1"/>
     <col min="40" max="40" width="10.7109375" style="3" customWidth="1"/>
+    <col min="41" max="41" width="17.7109375" style="3" customWidth="1"/>
+    <col min="42" max="42" width="12.7109375" style="3" customWidth="1"/>
+    <col min="43" max="43" width="21.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40">
+    <row r="1" spans="1:43">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="2" spans="1:40">
+        <v>129</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="2" spans="1:43">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2250,31 +2357,31 @@
         <v>6</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="3" spans="1:40">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="1:43">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -2282,7 +2389,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:40">
+    <row r="4" spans="1:43">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -2290,7 +2397,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:40">
+    <row r="5" spans="1:43">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -2298,16 +2405,16 @@
         <v>9</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="6" spans="1:40">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="6" spans="1:43">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -2315,22 +2422,22 @@
         <v>10</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="7" spans="1:40">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:43">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -2338,7 +2445,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:40">
+    <row r="8" spans="1:43">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -2346,25 +2453,25 @@
         <v>12</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="P8" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="Q8" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="R8" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="9" spans="1:40">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="9" spans="1:43">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -2372,7 +2479,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:40">
+    <row r="10" spans="1:43">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -2380,34 +2487,34 @@
         <v>14</v>
       </c>
       <c r="S10" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="T10" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="U10" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="V10" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="W10" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="X10" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="Y10" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="Z10" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="AA10" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="11" spans="1:40">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="11" spans="1:43">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -2415,19 +2522,19 @@
         <v>15</v>
       </c>
       <c r="AB11" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="AC11" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="AD11" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="AE11" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="12" spans="1:40">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="12" spans="1:43">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -2435,19 +2542,19 @@
         <v>16</v>
       </c>
       <c r="AF12" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="AG12" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="AH12" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="AI12" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="13" spans="1:40">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="13" spans="1:43">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -2455,16 +2562,16 @@
         <v>17</v>
       </c>
       <c r="AG13" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="AJ13" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="AK13" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="14" spans="1:40">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="14" spans="1:43">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -2472,134 +2579,169 @@
         <v>18</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="AL14" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="AM14" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="AN14" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="16" spans="1:40">
-      <c r="A16" t="s">
-        <v>126</v>
-      </c>
-      <c r="C16" s="3">
-        <v>1</v>
-      </c>
-      <c r="D16" s="3">
-        <v>1</v>
-      </c>
-      <c r="E16" s="3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="15" spans="1:43">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="M15" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="AO15" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="AP15" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="AQ15" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="17" spans="1:43">
+      <c r="A17" t="s">
+        <v>134</v>
+      </c>
+      <c r="C17" s="3">
+        <v>1</v>
+      </c>
+      <c r="D17" s="3">
+        <v>1</v>
+      </c>
+      <c r="E17" s="3">
+        <v>3</v>
+      </c>
+      <c r="F17" s="3">
+        <v>1</v>
+      </c>
+      <c r="G17" s="3">
         <v>2</v>
       </c>
-      <c r="F16" s="3">
-        <v>1</v>
-      </c>
-      <c r="G16" s="3">
-        <v>1</v>
-      </c>
-      <c r="H16" s="3">
-        <v>1</v>
-      </c>
-      <c r="I16" s="3">
-        <v>1</v>
-      </c>
-      <c r="J16" s="3">
-        <v>1</v>
-      </c>
-      <c r="K16" s="3">
+      <c r="H17" s="3">
+        <v>1</v>
+      </c>
+      <c r="I17" s="3">
+        <v>1</v>
+      </c>
+      <c r="J17" s="3">
+        <v>1</v>
+      </c>
+      <c r="K17" s="3">
         <v>2</v>
       </c>
-      <c r="L16" s="3">
-        <v>1</v>
-      </c>
-      <c r="M16" s="3">
-        <v>4</v>
-      </c>
-      <c r="N16" s="3">
+      <c r="L17" s="3">
+        <v>1</v>
+      </c>
+      <c r="M17" s="3">
+        <v>5</v>
+      </c>
+      <c r="N17" s="3">
         <v>2</v>
       </c>
-      <c r="O16" s="3">
-        <v>1</v>
-      </c>
-      <c r="P16" s="3">
+      <c r="O17" s="3">
+        <v>1</v>
+      </c>
+      <c r="P17" s="3">
         <v>2</v>
       </c>
-      <c r="Q16" s="3">
-        <v>1</v>
-      </c>
-      <c r="R16" s="3">
-        <v>1</v>
-      </c>
-      <c r="S16" s="3">
-        <v>1</v>
-      </c>
-      <c r="T16" s="3">
-        <v>1</v>
-      </c>
-      <c r="U16" s="3">
-        <v>1</v>
-      </c>
-      <c r="V16" s="3">
-        <v>1</v>
-      </c>
-      <c r="W16" s="3">
-        <v>1</v>
-      </c>
-      <c r="X16" s="3">
-        <v>1</v>
-      </c>
-      <c r="Y16" s="3">
-        <v>1</v>
-      </c>
-      <c r="Z16" s="3">
-        <v>1</v>
-      </c>
-      <c r="AA16" s="3">
-        <v>1</v>
-      </c>
-      <c r="AB16" s="3">
-        <v>1</v>
-      </c>
-      <c r="AC16" s="3">
-        <v>1</v>
-      </c>
-      <c r="AD16" s="3">
-        <v>1</v>
-      </c>
-      <c r="AE16" s="3">
-        <v>1</v>
-      </c>
-      <c r="AF16" s="3">
-        <v>1</v>
-      </c>
-      <c r="AG16" s="3">
+      <c r="Q17" s="3">
+        <v>1</v>
+      </c>
+      <c r="R17" s="3">
+        <v>1</v>
+      </c>
+      <c r="S17" s="3">
+        <v>1</v>
+      </c>
+      <c r="T17" s="3">
+        <v>1</v>
+      </c>
+      <c r="U17" s="3">
+        <v>1</v>
+      </c>
+      <c r="V17" s="3">
+        <v>1</v>
+      </c>
+      <c r="W17" s="3">
+        <v>1</v>
+      </c>
+      <c r="X17" s="3">
+        <v>1</v>
+      </c>
+      <c r="Y17" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z17" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA17" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB17" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC17" s="3">
+        <v>1</v>
+      </c>
+      <c r="AD17" s="3">
+        <v>1</v>
+      </c>
+      <c r="AE17" s="3">
+        <v>1</v>
+      </c>
+      <c r="AF17" s="3">
+        <v>1</v>
+      </c>
+      <c r="AG17" s="3">
         <v>2</v>
       </c>
-      <c r="AH16" s="3">
-        <v>1</v>
-      </c>
-      <c r="AI16" s="3">
-        <v>1</v>
-      </c>
-      <c r="AJ16" s="3">
-        <v>1</v>
-      </c>
-      <c r="AK16" s="3">
-        <v>1</v>
-      </c>
-      <c r="AL16" s="3">
-        <v>1</v>
-      </c>
-      <c r="AM16" s="3">
-        <v>1</v>
-      </c>
-      <c r="AN16" s="3">
+      <c r="AH17" s="3">
+        <v>1</v>
+      </c>
+      <c r="AI17" s="3">
+        <v>1</v>
+      </c>
+      <c r="AJ17" s="3">
+        <v>1</v>
+      </c>
+      <c r="AK17" s="3">
+        <v>1</v>
+      </c>
+      <c r="AL17" s="3">
+        <v>1</v>
+      </c>
+      <c r="AM17" s="3">
+        <v>1</v>
+      </c>
+      <c r="AN17" s="3">
+        <v>1</v>
+      </c>
+      <c r="AO17" s="3">
+        <v>1</v>
+      </c>
+      <c r="AP17" s="3">
+        <v>1</v>
+      </c>
+      <c r="AQ17" s="3">
         <v>1</v>
       </c>
     </row>
@@ -2610,7 +2752,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -2640,37 +2782,37 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -2681,19 +2823,19 @@
         <v>6</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -2702,6 +2844,9 @@
       </c>
       <c r="B3" t="s">
         <v>7</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -2711,9 +2856,6 @@
       <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>125</v>
-      </c>
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="1">
@@ -2723,10 +2865,10 @@
         <v>9</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -2737,7 +2879,7 @@
         <v>10</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -2756,13 +2898,13 @@
         <v>12</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -2781,10 +2923,10 @@
         <v>14</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -2795,7 +2937,7 @@
         <v>15</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
     </row>
     <row r="12" spans="1:13">
@@ -2806,7 +2948,7 @@
         <v>16</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
     </row>
     <row r="13" spans="1:13">
@@ -2817,16 +2959,16 @@
         <v>17</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
     </row>
     <row r="14" spans="1:13">
@@ -2837,56 +2979,67 @@
         <v>18</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13">
-      <c r="A16" t="s">
-        <v>126</v>
-      </c>
-      <c r="C16" s="3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" t="s">
+        <v>134</v>
+      </c>
+      <c r="C17" s="3">
         <v>2</v>
       </c>
-      <c r="D16" s="3">
-        <v>7</v>
-      </c>
-      <c r="E16" s="3">
+      <c r="D17" s="3">
+        <v>8</v>
+      </c>
+      <c r="E17" s="3">
         <v>2</v>
       </c>
-      <c r="F16" s="3">
-        <v>1</v>
-      </c>
-      <c r="G16" s="3">
+      <c r="F17" s="3">
+        <v>1</v>
+      </c>
+      <c r="G17" s="3">
         <v>4</v>
       </c>
-      <c r="H16" s="3">
+      <c r="H17" s="3">
         <v>3</v>
       </c>
-      <c r="I16" s="3">
-        <v>1</v>
-      </c>
-      <c r="J16" s="3">
+      <c r="I17" s="3">
+        <v>1</v>
+      </c>
+      <c r="J17" s="3">
         <v>2</v>
       </c>
-      <c r="K16" s="3">
-        <v>1</v>
-      </c>
-      <c r="L16" s="3">
-        <v>1</v>
-      </c>
-      <c r="M16" s="3">
+      <c r="K17" s="3">
+        <v>1</v>
+      </c>
+      <c r="L17" s="3">
+        <v>1</v>
+      </c>
+      <c r="M17" s="3">
         <v>1</v>
       </c>
     </row>
@@ -2897,7 +3050,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -2910,8 +3063,8 @@
   <cols>
     <col min="2" max="2" width="162.7109375" customWidth="1"/>
     <col min="3" max="3" width="25.7109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="35.7109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="35.7109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" style="3" customWidth="1"/>
     <col min="6" max="6" width="22.7109375" style="3" customWidth="1"/>
     <col min="7" max="7" width="13.7109375" style="3" customWidth="1"/>
     <col min="8" max="8" width="9.7109375" style="3" customWidth="1"/>
@@ -2924,28 +3077,28 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -2956,7 +3109,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -2967,7 +3120,7 @@
         <v>7</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -2978,7 +3131,7 @@
         <v>8</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -3005,7 +3158,7 @@
         <v>11</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -3024,10 +3177,10 @@
         <v>13</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -3038,10 +3191,10 @@
         <v>14</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -3060,7 +3213,7 @@
         <v>16</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -3079,32 +3232,40 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
-      <c r="A16" t="s">
-        <v>126</v>
-      </c>
-      <c r="C16" s="3">
-        <v>1</v>
-      </c>
-      <c r="D16" s="3">
-        <v>1</v>
-      </c>
-      <c r="E16" s="3">
-        <v>1</v>
-      </c>
-      <c r="F16" s="3">
+    <row r="15" spans="1:10">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" t="s">
+        <v>134</v>
+      </c>
+      <c r="C17" s="3">
+        <v>1</v>
+      </c>
+      <c r="D17" s="3">
+        <v>1</v>
+      </c>
+      <c r="E17" s="3">
+        <v>1</v>
+      </c>
+      <c r="F17" s="3">
         <v>2</v>
       </c>
-      <c r="G16" s="3">
-        <v>1</v>
-      </c>
-      <c r="H16" s="3">
-        <v>1</v>
-      </c>
-      <c r="I16" s="3">
-        <v>1</v>
-      </c>
-      <c r="J16" s="3">
+      <c r="G17" s="3">
+        <v>1</v>
+      </c>
+      <c r="H17" s="3">
+        <v>1</v>
+      </c>
+      <c r="I17" s="3">
+        <v>1</v>
+      </c>
+      <c r="J17" s="3">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Another paper processed 📖 Small corrections in other papers Improved script visual quality
</commit_message>
<xml_diff>
--- a/papers/stats/stats_spreadsheet.xlsx
+++ b/papers/stats/stats_spreadsheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="170">
   <si>
     <t>Paper Title</t>
   </si>
@@ -87,6 +87,9 @@
     <t>Automatic Analysis of the Emotional Content of Speech in Daylong Child-Centered Recordings from a Neonatal Intensive Care Unit</t>
   </si>
   <si>
+    <t>Lower speech connectedness linked to incidence of psychosis in people at clinical high risk</t>
+  </si>
+  <si>
     <t>Clemmer, Edward J.</t>
   </si>
   <si>
@@ -135,6 +138,9 @@
     <t>Vaaras E. Ahlqvist-Björkroth S. Drossos K et al</t>
   </si>
   <si>
+    <t>Spencer T. Thompson B. Oliver D. et al.</t>
+  </si>
+  <si>
     <t>1980</t>
   </si>
   <si>
@@ -315,6 +321,12 @@
     <t>Subject to Subject Evaluation</t>
   </si>
   <si>
+    <t>Word Graph Analysis</t>
+  </si>
+  <si>
+    <t>Comprehensive Assessment of At-Risk Mental States</t>
+  </si>
+  <si>
     <t>Speech Duration</t>
   </si>
   <si>
@@ -438,6 +450,24 @@
     <t>Duration of Utterance</t>
   </si>
   <si>
+    <t>Word Graph: Number of Edges</t>
+  </si>
+  <si>
+    <t>Word Graph: Number of Nodes in LCC</t>
+  </si>
+  <si>
+    <t>Word Graph: Number of nodes in LSC</t>
+  </si>
+  <si>
+    <t>Word Graph: Probability of LCC</t>
+  </si>
+  <si>
+    <t>Word Graph: Probability of LSC</t>
+  </si>
+  <si>
+    <t>Thought and Language Index</t>
+  </si>
+  <si>
     <t>X</t>
   </si>
   <si>
@@ -450,10 +480,10 @@
     <t>Small Sample</t>
   </si>
   <si>
-    <t>Schizophrenic under Medication</t>
-  </si>
-  <si>
-    <t>Schizophrenic under Lobotomy</t>
+    <t>Patients under Medication</t>
+  </si>
+  <si>
+    <t>Patients under Lobotomy</t>
   </si>
   <si>
     <t>Difference with other Neurological Disorders</t>
@@ -863,7 +893,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -910,10 +940,10 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E2" s="2">
         <v>44460</v>
@@ -933,10 +963,10 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E3" s="2">
         <v>44466</v>
@@ -956,10 +986,10 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E4" s="2">
         <v>44466</v>
@@ -979,10 +1009,10 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E5" s="2">
         <v>44468</v>
@@ -1002,10 +1032,10 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D6" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E6" s="2">
         <v>44470</v>
@@ -1025,10 +1055,10 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D7" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E7" s="2">
         <v>44471</v>
@@ -1048,10 +1078,10 @@
         <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E8" s="2">
         <v>44472</v>
@@ -1071,10 +1101,10 @@
         <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D9" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E9" s="2">
         <v>44473</v>
@@ -1094,10 +1124,10 @@
         <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D10" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E10" s="2">
         <v>44475</v>
@@ -1117,10 +1147,10 @@
         <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E11" s="2">
         <v>44477</v>
@@ -1140,10 +1170,10 @@
         <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D12" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E12" s="2">
         <v>44480</v>
@@ -1163,10 +1193,10 @@
         <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D13" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E13" s="2">
         <v>44483</v>
@@ -1186,10 +1216,10 @@
         <v>18</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D14" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E14" s="2">
         <v>44488</v>
@@ -1209,10 +1239,10 @@
         <v>19</v>
       </c>
       <c r="C15" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D15" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E15" s="2">
         <v>44488</v>
@@ -1232,10 +1262,10 @@
         <v>20</v>
       </c>
       <c r="C16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D16" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E16" s="2">
         <v>44489</v>
@@ -1255,10 +1285,10 @@
         <v>21</v>
       </c>
       <c r="C17" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D17" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E17" s="2">
         <v>44492</v>
@@ -1268,6 +1298,29 @@
       </c>
       <c r="G17">
         <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18" s="2">
+        <v>44492</v>
+      </c>
+      <c r="F18" s="2">
+        <v>44493</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1277,7 +1330,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T20"/>
+  <dimension ref="A1:T21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -1314,58 +1367,58 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:20">
@@ -1595,89 +1648,47 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:20">
-      <c r="A19" t="s">
-        <v>68</v>
-      </c>
-      <c r="C19" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="D19" s="3">
-        <v>1</v>
-      </c>
-      <c r="E19" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="F19" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="G19" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="H19" s="3">
-        <v>1</v>
-      </c>
-      <c r="I19" s="3">
-        <v>2</v>
-      </c>
-      <c r="J19" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="K19" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="L19" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="M19" s="3">
-        <v>4</v>
-      </c>
-      <c r="N19" s="3">
-        <v>2</v>
-      </c>
-      <c r="O19" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="P19" s="3">
-        <v>1</v>
-      </c>
-      <c r="Q19" s="3">
-        <v>2</v>
-      </c>
-      <c r="R19" s="3">
-        <v>1</v>
-      </c>
-      <c r="S19" s="3">
-        <v>1</v>
-      </c>
-      <c r="T19" s="3">
-        <v>2</v>
+    <row r="18" spans="1:20">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" s="3">
+        <v>1</v>
+      </c>
+      <c r="F18" s="3">
+        <v>1</v>
+      </c>
+      <c r="I18" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:20">
       <c r="A20" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C20" s="3">
-        <v>0.75</v>
+        <v>1.5</v>
       </c>
       <c r="D20" s="3">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E20" s="3">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="F20" s="3">
-        <v>0.75</v>
+        <v>2.5</v>
       </c>
       <c r="G20" s="3">
         <v>0.5</v>
       </c>
       <c r="H20" s="3">
-        <v>0.3333333333333333</v>
+        <v>1</v>
       </c>
       <c r="I20" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J20" s="3">
         <v>0.5</v>
@@ -1689,27 +1700,86 @@
         <v>0.5</v>
       </c>
       <c r="M20" s="3">
+        <v>4</v>
+      </c>
+      <c r="N20" s="3">
+        <v>2</v>
+      </c>
+      <c r="O20" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="P20" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q20" s="3">
+        <v>2</v>
+      </c>
+      <c r="R20" s="3">
+        <v>1</v>
+      </c>
+      <c r="S20" s="3">
+        <v>1</v>
+      </c>
+      <c r="T20" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20">
+      <c r="A21" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="D21" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="E21" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="F21" s="3">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="G21" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="H21" s="3">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="I21" s="3">
+        <v>1</v>
+      </c>
+      <c r="J21" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="K21" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="L21" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="M21" s="3">
         <v>0.8</v>
       </c>
-      <c r="N20" s="3">
+      <c r="N21" s="3">
         <v>0.6666666666666666</v>
       </c>
-      <c r="O20" s="3">
+      <c r="O21" s="3">
         <v>0.75</v>
       </c>
-      <c r="P20" s="3">
-        <v>1</v>
-      </c>
-      <c r="Q20" s="3">
-        <v>1</v>
-      </c>
-      <c r="R20" s="3">
-        <v>1</v>
-      </c>
-      <c r="S20" s="3">
-        <v>1</v>
-      </c>
-      <c r="T20" s="3">
+      <c r="P21" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q21" s="3">
+        <v>1</v>
+      </c>
+      <c r="R21" s="3">
+        <v>1</v>
+      </c>
+      <c r="S21" s="3">
+        <v>1</v>
+      </c>
+      <c r="T21" s="3">
         <v>1</v>
       </c>
     </row>
@@ -1720,7 +1790,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AD20"/>
+  <dimension ref="A1:AF21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -1760,98 +1830,106 @@
     <col min="28" max="28" width="11.7109375" style="3" customWidth="1"/>
     <col min="29" max="29" width="20.7109375" style="3" customWidth="1"/>
     <col min="30" max="30" width="29.7109375" style="3" customWidth="1"/>
+    <col min="31" max="31" width="19.7109375" style="3" customWidth="1"/>
+    <col min="32" max="32" width="49.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30">
+    <row r="1" spans="1:32">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="2" spans="1:30">
+        <v>99</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1871,7 +1949,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:30">
+    <row r="3" spans="1:32">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1879,7 +1957,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:30">
+    <row r="4" spans="1:32">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1887,7 +1965,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:30">
+    <row r="5" spans="1:32">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1907,7 +1985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:30">
+    <row r="6" spans="1:32">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1921,7 +1999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:30">
+    <row r="7" spans="1:32">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1929,7 +2007,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:30">
+    <row r="8" spans="1:32">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1949,7 +2027,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:30">
+    <row r="9" spans="1:32">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1960,7 +2038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:30">
+    <row r="10" spans="1:32">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1977,7 +2055,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:30">
+    <row r="11" spans="1:32">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -2003,7 +2081,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:30">
+    <row r="12" spans="1:32">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -2026,7 +2104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:30">
+    <row r="13" spans="1:32">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -2046,7 +2124,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:30">
+    <row r="14" spans="1:32">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -2057,7 +2135,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:30">
+    <row r="15" spans="1:32">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -2071,7 +2149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:30">
+    <row r="16" spans="1:32">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -2082,7 +2160,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:30">
+    <row r="17" spans="1:32">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -2090,107 +2168,41 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:30">
-      <c r="A19" t="s">
-        <v>68</v>
-      </c>
-      <c r="C19" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="D19" s="3">
-        <v>1</v>
-      </c>
-      <c r="E19" s="3">
+    <row r="18" spans="1:32">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="3">
+        <v>1</v>
+      </c>
+      <c r="K18" s="3">
+        <v>1</v>
+      </c>
+      <c r="S18" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AE18" s="3">
+        <v>1</v>
+      </c>
+      <c r="AF18" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:32">
+      <c r="A20" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="D20" s="3">
+        <v>1</v>
+      </c>
+      <c r="E20" s="3">
         <v>2</v>
-      </c>
-      <c r="F19" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="G19" s="3">
-        <v>1</v>
-      </c>
-      <c r="H19" s="3">
-        <v>1</v>
-      </c>
-      <c r="I19" s="3">
-        <v>1</v>
-      </c>
-      <c r="J19" s="3">
-        <v>1</v>
-      </c>
-      <c r="K19" s="3">
-        <v>1</v>
-      </c>
-      <c r="L19" s="3">
-        <v>1</v>
-      </c>
-      <c r="M19" s="3">
-        <v>1</v>
-      </c>
-      <c r="N19" s="3">
-        <v>0</v>
-      </c>
-      <c r="O19" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="P19" s="3">
-        <v>3</v>
-      </c>
-      <c r="Q19" s="3">
-        <v>1</v>
-      </c>
-      <c r="R19" s="3">
-        <v>1</v>
-      </c>
-      <c r="S19" s="3">
-        <v>3</v>
-      </c>
-      <c r="T19" s="3">
-        <v>2</v>
-      </c>
-      <c r="U19" s="3">
-        <v>1</v>
-      </c>
-      <c r="V19" s="3">
-        <v>1</v>
-      </c>
-      <c r="W19" s="3">
-        <v>2</v>
-      </c>
-      <c r="X19" s="3">
-        <v>1</v>
-      </c>
-      <c r="Y19" s="3">
-        <v>1</v>
-      </c>
-      <c r="Z19" s="3">
-        <v>1</v>
-      </c>
-      <c r="AA19" s="3">
-        <v>1</v>
-      </c>
-      <c r="AB19" s="3">
-        <v>1</v>
-      </c>
-      <c r="AC19" s="3">
-        <v>1</v>
-      </c>
-      <c r="AD19" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:30">
-      <c r="A20" t="s">
-        <v>69</v>
-      </c>
-      <c r="C20" s="3">
-        <v>0.75</v>
-      </c>
-      <c r="D20" s="3">
-        <v>1</v>
-      </c>
-      <c r="E20" s="3">
-        <v>1</v>
       </c>
       <c r="F20" s="3">
         <v>0.5</v>
@@ -2208,7 +2220,7 @@
         <v>1</v>
       </c>
       <c r="K20" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L20" s="3">
         <v>1</v>
@@ -2220,52 +2232,153 @@
         <v>0</v>
       </c>
       <c r="O20" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="P20" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q20" s="3">
+        <v>1</v>
+      </c>
+      <c r="R20" s="3">
+        <v>1</v>
+      </c>
+      <c r="S20" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="T20" s="3">
+        <v>2</v>
+      </c>
+      <c r="U20" s="3">
+        <v>1</v>
+      </c>
+      <c r="V20" s="3">
+        <v>1</v>
+      </c>
+      <c r="W20" s="3">
+        <v>2</v>
+      </c>
+      <c r="X20" s="3">
+        <v>1</v>
+      </c>
+      <c r="Y20" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z20" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA20" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB20" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC20" s="3">
+        <v>1</v>
+      </c>
+      <c r="AD20" s="3">
+        <v>1</v>
+      </c>
+      <c r="AE20" s="3">
+        <v>1</v>
+      </c>
+      <c r="AF20" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:32">
+      <c r="A21" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" s="3">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="D21" s="3">
+        <v>1</v>
+      </c>
+      <c r="E21" s="3">
+        <v>1</v>
+      </c>
+      <c r="F21" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G21" s="3">
+        <v>1</v>
+      </c>
+      <c r="H21" s="3">
+        <v>1</v>
+      </c>
+      <c r="I21" s="3">
+        <v>1</v>
+      </c>
+      <c r="J21" s="3">
+        <v>1</v>
+      </c>
+      <c r="K21" s="3">
+        <v>1</v>
+      </c>
+      <c r="L21" s="3">
+        <v>1</v>
+      </c>
+      <c r="M21" s="3">
+        <v>1</v>
+      </c>
+      <c r="N21" s="3">
+        <v>0</v>
+      </c>
+      <c r="O21" s="3">
         <v>0.75</v>
       </c>
-      <c r="P20" s="3">
-        <v>1</v>
-      </c>
-      <c r="Q20" s="3">
-        <v>1</v>
-      </c>
-      <c r="R20" s="3">
-        <v>1</v>
-      </c>
-      <c r="S20" s="3">
-        <v>1</v>
-      </c>
-      <c r="T20" s="3">
-        <v>1</v>
-      </c>
-      <c r="U20" s="3">
-        <v>1</v>
-      </c>
-      <c r="V20" s="3">
-        <v>1</v>
-      </c>
-      <c r="W20" s="3">
-        <v>1</v>
-      </c>
-      <c r="X20" s="3">
-        <v>1</v>
-      </c>
-      <c r="Y20" s="3">
-        <v>1</v>
-      </c>
-      <c r="Z20" s="3">
-        <v>1</v>
-      </c>
-      <c r="AA20" s="3">
-        <v>1</v>
-      </c>
-      <c r="AB20" s="3">
-        <v>1</v>
-      </c>
-      <c r="AC20" s="3">
-        <v>1</v>
-      </c>
-      <c r="AD20" s="3">
-        <v>1</v>
+      <c r="P21" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q21" s="3">
+        <v>1</v>
+      </c>
+      <c r="R21" s="3">
+        <v>1</v>
+      </c>
+      <c r="S21" s="3">
+        <v>0.875</v>
+      </c>
+      <c r="T21" s="3">
+        <v>1</v>
+      </c>
+      <c r="U21" s="3">
+        <v>1</v>
+      </c>
+      <c r="V21" s="3">
+        <v>1</v>
+      </c>
+      <c r="W21" s="3">
+        <v>1</v>
+      </c>
+      <c r="X21" s="3">
+        <v>1</v>
+      </c>
+      <c r="Y21" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z21" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA21" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB21" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC21" s="3">
+        <v>1</v>
+      </c>
+      <c r="AD21" s="3">
+        <v>1</v>
+      </c>
+      <c r="AE21" s="3">
+        <v>1</v>
+      </c>
+      <c r="AF21" s="3">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>
@@ -2275,7 +2388,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AQ19"/>
+  <dimension ref="A1:AW20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -2328,137 +2441,161 @@
     <col min="41" max="41" width="17.7109375" style="3" customWidth="1"/>
     <col min="42" max="42" width="12.7109375" style="3" customWidth="1"/>
     <col min="43" max="43" width="21.7109375" style="3" customWidth="1"/>
+    <col min="44" max="44" width="27.7109375" style="3" customWidth="1"/>
+    <col min="45" max="45" width="34.7109375" style="3" customWidth="1"/>
+    <col min="46" max="46" width="34.7109375" style="3" customWidth="1"/>
+    <col min="47" max="47" width="30.7109375" style="3" customWidth="1"/>
+    <col min="48" max="48" width="30.7109375" style="3" customWidth="1"/>
+    <col min="49" max="49" width="26.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43">
+    <row r="1" spans="1:49">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="AQ1" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="2" spans="1:43">
+        <v>142</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="1:49">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2466,31 +2603,31 @@
         <v>6</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="3" spans="1:43">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="3" spans="1:49">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -2498,7 +2635,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:43">
+    <row r="4" spans="1:49">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -2506,7 +2643,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:43">
+    <row r="5" spans="1:49">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -2514,16 +2651,16 @@
         <v>9</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="6" spans="1:43">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="6" spans="1:49">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -2531,22 +2668,22 @@
         <v>10</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="7" spans="1:43">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="7" spans="1:49">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -2554,7 +2691,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:43">
+    <row r="8" spans="1:49">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -2562,25 +2699,25 @@
         <v>12</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="P8" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="Q8" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="R8" s="3" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="9" spans="1:43">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="9" spans="1:49">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -2588,7 +2725,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:43">
+    <row r="10" spans="1:49">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -2596,34 +2733,34 @@
         <v>14</v>
       </c>
       <c r="S10" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="T10" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="U10" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="V10" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="W10" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="X10" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="Y10" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="Z10" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="AA10" s="3" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="11" spans="1:43">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="11" spans="1:49">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -2631,19 +2768,19 @@
         <v>15</v>
       </c>
       <c r="AB11" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="AC11" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="AD11" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="AE11" s="3" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="12" spans="1:43">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="12" spans="1:49">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -2651,19 +2788,19 @@
         <v>16</v>
       </c>
       <c r="AF12" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="AG12" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="AH12" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="AI12" s="3" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="13" spans="1:43">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="13" spans="1:49">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -2671,16 +2808,16 @@
         <v>17</v>
       </c>
       <c r="AG13" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="AJ13" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="AK13" s="3" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="14" spans="1:43">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="14" spans="1:49">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -2688,19 +2825,19 @@
         <v>18</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="AL14" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="AM14" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="AN14" s="3" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="15" spans="1:43">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="15" spans="1:49">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -2708,25 +2845,25 @@
         <v>19</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="AO15" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="AP15" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="AQ15" s="3" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="16" spans="1:43">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="16" spans="1:49">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -2734,7 +2871,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:43">
+    <row r="17" spans="1:49">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -2742,131 +2879,178 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:43">
-      <c r="A19" t="s">
-        <v>140</v>
-      </c>
-      <c r="C19" s="3">
-        <v>1</v>
-      </c>
-      <c r="D19" s="3">
-        <v>1</v>
-      </c>
-      <c r="E19" s="3">
+    <row r="18" spans="1:49">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="M18" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="AR18" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="AS18" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="AT18" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="AU18" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="AV18" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="AW18" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="20" spans="1:49">
+      <c r="A20" t="s">
+        <v>150</v>
+      </c>
+      <c r="C20" s="3">
+        <v>1</v>
+      </c>
+      <c r="D20" s="3">
+        <v>1</v>
+      </c>
+      <c r="E20" s="3">
         <v>3</v>
       </c>
-      <c r="F19" s="3">
-        <v>1</v>
-      </c>
-      <c r="G19" s="3">
+      <c r="F20" s="3">
+        <v>1</v>
+      </c>
+      <c r="G20" s="3">
         <v>2</v>
       </c>
-      <c r="H19" s="3">
-        <v>1</v>
-      </c>
-      <c r="I19" s="3">
-        <v>1</v>
-      </c>
-      <c r="J19" s="3">
-        <v>1</v>
-      </c>
-      <c r="K19" s="3">
+      <c r="H20" s="3">
+        <v>1</v>
+      </c>
+      <c r="I20" s="3">
+        <v>1</v>
+      </c>
+      <c r="J20" s="3">
+        <v>1</v>
+      </c>
+      <c r="K20" s="3">
         <v>2</v>
       </c>
-      <c r="L19" s="3">
-        <v>1</v>
-      </c>
-      <c r="M19" s="3">
-        <v>5</v>
-      </c>
-      <c r="N19" s="3">
+      <c r="L20" s="3">
+        <v>1</v>
+      </c>
+      <c r="M20" s="3">
+        <v>6</v>
+      </c>
+      <c r="N20" s="3">
         <v>2</v>
       </c>
-      <c r="O19" s="3">
-        <v>1</v>
-      </c>
-      <c r="P19" s="3">
+      <c r="O20" s="3">
+        <v>1</v>
+      </c>
+      <c r="P20" s="3">
         <v>2</v>
       </c>
-      <c r="Q19" s="3">
-        <v>1</v>
-      </c>
-      <c r="R19" s="3">
-        <v>1</v>
-      </c>
-      <c r="S19" s="3">
-        <v>1</v>
-      </c>
-      <c r="T19" s="3">
-        <v>1</v>
-      </c>
-      <c r="U19" s="3">
-        <v>1</v>
-      </c>
-      <c r="V19" s="3">
-        <v>1</v>
-      </c>
-      <c r="W19" s="3">
-        <v>1</v>
-      </c>
-      <c r="X19" s="3">
-        <v>1</v>
-      </c>
-      <c r="Y19" s="3">
-        <v>1</v>
-      </c>
-      <c r="Z19" s="3">
-        <v>1</v>
-      </c>
-      <c r="AA19" s="3">
-        <v>1</v>
-      </c>
-      <c r="AB19" s="3">
-        <v>1</v>
-      </c>
-      <c r="AC19" s="3">
-        <v>1</v>
-      </c>
-      <c r="AD19" s="3">
-        <v>1</v>
-      </c>
-      <c r="AE19" s="3">
-        <v>1</v>
-      </c>
-      <c r="AF19" s="3">
-        <v>1</v>
-      </c>
-      <c r="AG19" s="3">
+      <c r="Q20" s="3">
+        <v>1</v>
+      </c>
+      <c r="R20" s="3">
+        <v>1</v>
+      </c>
+      <c r="S20" s="3">
+        <v>1</v>
+      </c>
+      <c r="T20" s="3">
+        <v>1</v>
+      </c>
+      <c r="U20" s="3">
+        <v>1</v>
+      </c>
+      <c r="V20" s="3">
+        <v>1</v>
+      </c>
+      <c r="W20" s="3">
+        <v>1</v>
+      </c>
+      <c r="X20" s="3">
+        <v>1</v>
+      </c>
+      <c r="Y20" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z20" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA20" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB20" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC20" s="3">
+        <v>1</v>
+      </c>
+      <c r="AD20" s="3">
+        <v>1</v>
+      </c>
+      <c r="AE20" s="3">
+        <v>1</v>
+      </c>
+      <c r="AF20" s="3">
+        <v>1</v>
+      </c>
+      <c r="AG20" s="3">
         <v>2</v>
       </c>
-      <c r="AH19" s="3">
-        <v>1</v>
-      </c>
-      <c r="AI19" s="3">
-        <v>1</v>
-      </c>
-      <c r="AJ19" s="3">
-        <v>1</v>
-      </c>
-      <c r="AK19" s="3">
-        <v>1</v>
-      </c>
-      <c r="AL19" s="3">
-        <v>1</v>
-      </c>
-      <c r="AM19" s="3">
-        <v>1</v>
-      </c>
-      <c r="AN19" s="3">
-        <v>1</v>
-      </c>
-      <c r="AO19" s="3">
-        <v>1</v>
-      </c>
-      <c r="AP19" s="3">
-        <v>1</v>
-      </c>
-      <c r="AQ19" s="3">
+      <c r="AH20" s="3">
+        <v>1</v>
+      </c>
+      <c r="AI20" s="3">
+        <v>1</v>
+      </c>
+      <c r="AJ20" s="3">
+        <v>1</v>
+      </c>
+      <c r="AK20" s="3">
+        <v>1</v>
+      </c>
+      <c r="AL20" s="3">
+        <v>1</v>
+      </c>
+      <c r="AM20" s="3">
+        <v>1</v>
+      </c>
+      <c r="AN20" s="3">
+        <v>1</v>
+      </c>
+      <c r="AO20" s="3">
+        <v>1</v>
+      </c>
+      <c r="AP20" s="3">
+        <v>1</v>
+      </c>
+      <c r="AQ20" s="3">
+        <v>1</v>
+      </c>
+      <c r="AR20" s="3">
+        <v>1</v>
+      </c>
+      <c r="AS20" s="3">
+        <v>1</v>
+      </c>
+      <c r="AT20" s="3">
+        <v>1</v>
+      </c>
+      <c r="AU20" s="3">
+        <v>1</v>
+      </c>
+      <c r="AV20" s="3">
+        <v>1</v>
+      </c>
+      <c r="AW20" s="3">
         <v>1</v>
       </c>
     </row>
@@ -2877,7 +3061,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M19"/>
+  <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -2891,8 +3075,8 @@
     <col min="2" max="2" width="162.7109375" customWidth="1"/>
     <col min="3" max="3" width="18.7109375" style="3" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="30.7109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="28.7109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="23.7109375" style="3" customWidth="1"/>
     <col min="7" max="7" width="44.7109375" style="3" customWidth="1"/>
     <col min="8" max="8" width="16.7109375" style="3" customWidth="1"/>
     <col min="9" max="9" width="22.7109375" style="3" customWidth="1"/>
@@ -2907,37 +3091,37 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>142</v>
+        <v>152</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>147</v>
+        <v>157</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -2948,19 +3132,19 @@
         <v>6</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -2971,7 +3155,7 @@
         <v>7</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -2990,10 +3174,10 @@
         <v>9</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -3004,7 +3188,7 @@
         <v>10</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -3023,13 +3207,13 @@
         <v>12</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -3048,10 +3232,10 @@
         <v>14</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -3062,7 +3246,7 @@
         <v>15</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
     </row>
     <row r="12" spans="1:13">
@@ -3073,7 +3257,7 @@
         <v>16</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
     </row>
     <row r="13" spans="1:13">
@@ -3084,16 +3268,16 @@
         <v>17</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
     </row>
     <row r="14" spans="1:13">
@@ -3104,19 +3288,19 @@
         <v>18</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
     </row>
     <row r="15" spans="1:13">
@@ -3127,7 +3311,7 @@
         <v>19</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
     </row>
     <row r="16" spans="1:13">
@@ -3146,41 +3330,55 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
-      <c r="A19" t="s">
-        <v>140</v>
-      </c>
-      <c r="C19" s="3">
+    <row r="18" spans="1:13">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20" t="s">
+        <v>150</v>
+      </c>
+      <c r="C20" s="3">
         <v>2</v>
       </c>
-      <c r="D19" s="3">
-        <v>8</v>
-      </c>
-      <c r="E19" s="3">
+      <c r="D20" s="3">
+        <v>9</v>
+      </c>
+      <c r="E20" s="3">
+        <v>3</v>
+      </c>
+      <c r="F20" s="3">
+        <v>1</v>
+      </c>
+      <c r="G20" s="3">
+        <v>4</v>
+      </c>
+      <c r="H20" s="3">
+        <v>3</v>
+      </c>
+      <c r="I20" s="3">
+        <v>1</v>
+      </c>
+      <c r="J20" s="3">
         <v>2</v>
       </c>
-      <c r="F19" s="3">
-        <v>1</v>
-      </c>
-      <c r="G19" s="3">
-        <v>4</v>
-      </c>
-      <c r="H19" s="3">
-        <v>3</v>
-      </c>
-      <c r="I19" s="3">
-        <v>1</v>
-      </c>
-      <c r="J19" s="3">
-        <v>2</v>
-      </c>
-      <c r="K19" s="3">
-        <v>1</v>
-      </c>
-      <c r="L19" s="3">
-        <v>1</v>
-      </c>
-      <c r="M19" s="3">
+      <c r="K20" s="3">
+        <v>1</v>
+      </c>
+      <c r="L20" s="3">
+        <v>1</v>
+      </c>
+      <c r="M20" s="3">
         <v>1</v>
       </c>
     </row>
@@ -3191,7 +3389,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -3218,28 +3416,28 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>159</v>
+        <v>169</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -3250,7 +3448,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -3261,7 +3459,7 @@
         <v>7</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -3272,7 +3470,7 @@
         <v>8</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -3299,7 +3497,7 @@
         <v>11</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -3318,10 +3516,10 @@
         <v>13</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -3332,10 +3530,10 @@
         <v>14</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -3354,7 +3552,7 @@
         <v>16</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -3397,32 +3595,40 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
-      <c r="A19" t="s">
-        <v>140</v>
-      </c>
-      <c r="C19" s="3">
-        <v>1</v>
-      </c>
-      <c r="D19" s="3">
-        <v>1</v>
-      </c>
-      <c r="E19" s="3">
-        <v>1</v>
-      </c>
-      <c r="F19" s="3">
+    <row r="18" spans="1:10">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" t="s">
+        <v>150</v>
+      </c>
+      <c r="C20" s="3">
+        <v>1</v>
+      </c>
+      <c r="D20" s="3">
+        <v>1</v>
+      </c>
+      <c r="E20" s="3">
+        <v>1</v>
+      </c>
+      <c r="F20" s="3">
         <v>2</v>
       </c>
-      <c r="G19" s="3">
-        <v>1</v>
-      </c>
-      <c r="H19" s="3">
-        <v>1</v>
-      </c>
-      <c r="I19" s="3">
-        <v>1</v>
-      </c>
-      <c r="J19" s="3">
+      <c r="G20" s="3">
+        <v>1</v>
+      </c>
+      <c r="H20" s="3">
+        <v>1</v>
+      </c>
+      <c r="I20" s="3">
+        <v>1</v>
+      </c>
+      <c r="J20" s="3">
         <v>1</v>
       </c>
     </row>

</xml_diff>